<commit_message>
rules for later sessions
</commit_message>
<xml_diff>
--- a/actions/Activities.xlsx
+++ b/actions/Activities.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-120" windowWidth="19200" windowHeight="5520" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="-120" windowWidth="19200" windowHeight="5520"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="6" r:id="rId1"/>
@@ -582,13 +582,7 @@
     <t>When preparing for quitting smoking, it can help to learn from other people who have successfully quit smoking. What motivated them to quit? And what helped them to succeed? Before the next session, I thus recommend you watch two short videos with tips from former smokers. First this 2-minute video in which Brett tells you about how he quit smoking for a healthier future: https://www.youtube.com/watch?v=SkxajRN4Fho&amp;ab_channel=CentersforDiseaseControlandPrevention%28CDC%29. And then this short video in which Tiffany tells you how she quit smoking: https://www.youtube.com/watch?v=6OZehKDHsj0&amp;ab_channel=CentersforDiseaseControlandPrevention%28CDC%29. What can you take away from these two examples for yourself? Take a few notes on your phone or a piece of paper.</t>
   </si>
   <si>
-    <t>When preparing for becoming more physically active, it can be useful to learn from other people who have succeeded in becoming more physically active. What goal did they set for themselves? And how did they reach it? Before the next session, I thus recommend you watch this short video in which 5 people describe how they reached their physical activity goals: &lt;insert link&gt;. What can you take away from the 5 examples for yourself? Take a few notes on a piece of paper or your phone.</t>
-  </si>
-  <si>
     <t>https://www.cdc.gov/tobacco/campaign/tips/stories/index.html</t>
-  </si>
-  <si>
-    <t>Becoming more physically active (e.g., swimming, taking walks, boxing) may help you to successfully quit smoking. One crucial step for this is to have high aspiration to become more physically active. So, before the next session, I advise you to watch the following short video about the possible positive impact of physical activity on dealing with cravings to smoke: &lt;insert our link&gt;. What do you think about the information in the video? Write down your thoughts in a few words.</t>
   </si>
   <si>
     <t>Having strong motivation to quit smoking helps to quit successfully. Before the next session, I thus suggest you take some time to look for a motivational quote or write down something that motivates you to quit smoking. Place this somewhere you can see it every day, such as your fridge or closet door.</t>
@@ -1484,24 +1478,6 @@
     <t>Adopting the right mindset is crucial in altering one's behavior. It involves identifying the desired end result and having faith in one's ability to attain it. Adequate motivation and self-confidence are crucial in this process. To see why, I recommend watching this short video before the next session: &lt;insert our link&gt;. What do you think, how can self-confidence and motivation help you to reach your end goal? Write down your thoughts on a piece of paper or your phone.</t>
   </si>
   <si>
-    <t>Some very practical steps can aid in effectively changing your behavior. This includes acquiring an understanding of your current behavior, exploring strategies to overcome possible obstacles, and preparing things that will motivate you. To see why, I advise watching this short video before the next session: &lt;insert our link&gt;. How do you think practical preparations can help you become more physically active and quit smoking? Write down your thoughts on a piece of paper or your phone.</t>
-  </si>
-  <si>
-    <t>Keeping a positive outlook and being aware of positive outcomes of one's behavior change can help to overcome possible obstacles. To see why, I recommend watching this short video before the next session: &lt;insert our link&gt;. How do you think that thinking about "positive" things can help you to become more physically active and quit smoking? Note your thoughts on your phone or a piece of paper.</t>
-  </si>
-  <si>
-    <t>When preparing for changing your behavior, it is helpful to think about 3 types of "negative" things. This includes obstacles, possible short-term adverse effects on your well-being, and things that could happen in the future if you do not change. To see why, I advise watching this short video before the next session: &lt;insert our link&gt;. How can thinking about "negative" things help you to become more physically active and quit smoking? Note your thoughts on your phone or a piece of paper.</t>
-  </si>
-  <si>
-    <t>Motivation is crucial when changing your behavior. To see why, I suggest watching this short video before the next session: &lt;insert our link&gt;. What do you think, how can (more) motivation help you quit smoking and become more physically active? Write down your thoughts on a piece of paper or your phone.</t>
-  </si>
-  <si>
-    <t>Knowledge of how to manage cravings and the often associated negative feelings such as anger, frustration, irritability, or anxiety helps to quit smoking successfully. To see why, I suggest watching this short video before the next session: &lt;insert our link&gt;. How do you think can knowledge of how to manage cravings and the resulting negative feelings help you quit smoking? Note your thoughts on a piece of paper or your phone.</t>
-  </si>
-  <si>
-    <t>Physical activity helps to quit smoking. To see why, I suggest watching this short video before the next session: &lt;insert our link&gt;. How do you think can physical activity help you to quit smoking? Collect your ideas on a piece of paper or your phone.</t>
-  </si>
-  <si>
     <t>Adopting the right mindset is crucial in altering one's behavior. It involves identifying the desired end result and having faith in one's ability to attain it. Adequate motivation and self-confidence are crucial in this process. To see why, I recommend watching the short video that I will send you in a message on Prolific right after this session. What do you think, how can self-confidence and motivation help you to reach your end goal? Write down your thoughts on a piece of paper or your phone.</t>
   </si>
   <si>
@@ -1907,9 +1883,6 @@
     <t>It is possible that people who quit smoking gain some weight. Learning how you can maintain a healthy weight after quitting smoking can help you to quit and stay quit. I, therefore, recommend watching a short video with tips on how to prevent a large weight gain after quitting smoking. I will send you the link to the video in a message on Prolific right after this session. After watching the video, think about what you can take away from these tips for maintaining a healthy weight after quitting smoking for yourself. Grab a pen and piece of paper and note your takeaways.</t>
   </si>
   <si>
-    <t>It is possible that people who quit smoking gain some weight. Learning how you can maintain a healthy weight after quitting smoking can help you to quit and stay quit. I, therefore, recommend watching this short video with tips on how to prevent a large weight gain after quitting smoking before the next session: &lt;insert our link&gt;. What can you take away from these tips for maintaining a healthy weight after quitting smoking for yourself? Grab a pen and piece of paper and note your takeaways.</t>
-  </si>
-  <si>
     <t>This activity is called "Positive Diary" and helps you think positively and feel good. This can help you quit smoking and become more physically active. In the evening before going to bed, think about the day you had. Write down 2 or 3 things that happened that you are grateful for, happy about, or that went well. For example, "Someone smiled at me in the supermarket," "I did not smoke today," or "I took a nice walk with a friend." Writing down these positive moments can help you feel better, about yourself and about your day. You can write down anything! It does not have to be about being more physically active or quitting smoking, but can be any enjoyable moment from the day, big or small. This will help you to focus on positive things.</t>
   </si>
   <si>
@@ -1922,15 +1895,9 @@
     <t>It is common for individuals to encounter barriers or obstacles that make it more difficult for them to change their behavior. For example, a lack of support from one's friends for quitting smoking. Or not having running shoes. When preparing to change one's behavior, it is advantageous to consider potential obstacles to successfully changing one's behavior. To see why, I suggest watching the short video that I will send you in a message on Prolific right after this session. How do you think can thinking of possible obstacles help you to quit smoking and become more physically active? Collect your thoughts on your phone or a piece of paper.</t>
   </si>
   <si>
-    <t>It is common for individuals to encounter barriers or obstacles that make it more difficult for them to change their behavior. For example, a lack of support from one's friends for quitting smoking. Or not having running shoes. When preparing to change one's behavior, it is advantageous to consider potential obstacles to successfully changing one's behavior. To see why, I suggest watching this short video before the next session: &lt;insert our link&gt;. How do you think can thinking of possible obstacles help you to quit smoking and become more physically active? Collect your thoughts on your phone or a piece of paper.</t>
-  </si>
-  <si>
     <t>When changing one's behavior, it is possible that in the short term, one's mental and/or physical well-being decline. For example, you may sleep worse for some time after quitting smoking. Such negative effects can make it challenging to both begin and sustain the behavior change. But there are steps that you can take to minimize or even prevent such negative effects. To learn more, I advise watching the short video that I will send you in a message on Prolific right after this session. What do you think, how can learning about steps to reduce short-term negative effects on your mental and physical well-being help you to quit smoking and become more physically active? Note your thoughts on your phone or a piece of paper.</t>
   </si>
   <si>
-    <t>When changing one's behavior, it is possible that in the short term, one's mental and/or physical well-being decline. For example, you may sleep worse for some time after quitting smoking. Such negative effects can make it challenging to both begin and sustain the behavior change. But there are steps that you can take to minimize or even prevent such negative effects. To learn more, I advise watching this short video before the next session: &lt;insert our link&gt;. What do you think, how can learning about steps to reduce short-term negative effects on your mental and physical well-being help you to quit smoking and become more physically active? Note your thoughts on your phone or a piece of paper.</t>
-  </si>
-  <si>
     <t>Thinking about how quitting smoking makes one a role model by doing something good for others (e.g., children or friends).</t>
   </si>
   <si>
@@ -1938,6 +1905,39 @@
   </si>
   <si>
     <t>Most exclusions are the same as in the first experiment. But then people were also supposed to only watch one video for PA and one video for smoking. So that meant that people would only either learn about recommended PA or about how PA impacts cravings to smoke, for example. We removed these exclusions. We also added one more future selves exercise (we only had 3 for smoking in the first experiment), which is included in the corresponding exclusion criteria on doing only one feared and only one desired future selves exercise.</t>
+  </si>
+  <si>
+    <t>It is possible that people who quit smoking gain some weight. Learning how you can maintain a healthy weight after quitting smoking can help you to quit and stay quit. I, therefore, recommend watching this short video with tips on how to prevent a large weight gain after quitting smoking before the next session: https://youtu.be/jseVEv9tVS8. What can you take away from these tips for maintaining a healthy weight after quitting smoking for yourself? Grab a pen and piece of paper and note your takeaways.</t>
+  </si>
+  <si>
+    <t>Becoming more physically active (e.g., swimming, taking walks, boxing) may help you to successfully quit smoking. One crucial step for this is to have high aspiration to become more physically active. So, before the next session, I advise you to watch the following short video about the possible positive impact of physical activity on dealing with cravings to smoke: https://youtu.be/iakhFA-jPCc. What do you think about the information in the video? Write down your thoughts in a few words.</t>
+  </si>
+  <si>
+    <t>Some very practical steps can aid in effectively changing your behavior. This includes acquiring an understanding of your current behavior, exploring strategies to overcome possible obstacles, and preparing things that will motivate you. To see why, I advise watching this short video before the next session: https://youtu.be/CM_u7oV7WXU. How do you think practical preparations can help you become more physically active and quit smoking? Write down your thoughts on a piece of paper or your phone.</t>
+  </si>
+  <si>
+    <t>Keeping a positive outlook and being aware of positive outcomes of one's behavior change can help to overcome possible obstacles. To see why, I recommend watching this short video before the next session: https://youtu.be/_BnMm3EKrDk. How do you think that thinking about "positive" things can help you to become more physically active and quit smoking? Note your thoughts on your phone or a piece of paper.</t>
+  </si>
+  <si>
+    <t>When preparing for changing your behavior, it is helpful to think about 3 types of "negative" things. This includes obstacles, possible short-term adverse effects on your well-being, and things that could happen in the future if you do not change. To see why, I advise watching this short video before the next session: https://youtu.be/28ggci50PvU. How can thinking about "negative" things help you to become more physically active and quit smoking? Note your thoughts on your phone or a piece of paper.</t>
+  </si>
+  <si>
+    <t>Motivation is crucial when changing your behavior. To see why, I suggest watching this short video before the next session: https://youtu.be/kEadOY713qs. What do you think, how can (more) motivation help you quit smoking and become more physically active? Write down your thoughts on a piece of paper or your phone.</t>
+  </si>
+  <si>
+    <t>Knowledge of how to manage cravings and the often associated negative feelings such as anger, frustration, irritability, or anxiety helps to quit smoking successfully. To see why, I suggest watching this short video before the next session: https://youtu.be/_pTTeIaObHc. How do you think can knowledge of how to manage cravings and the resulting negative feelings help you quit smoking? Note your thoughts on a piece of paper or your phone.</t>
+  </si>
+  <si>
+    <t>Physical activity helps to quit smoking. To see why, I suggest watching this short video before the next session: https://youtu.be/qoD2j_lTm9U. How do you think can physical activity help you to quit smoking? Collect your ideas on a piece of paper or your phone.</t>
+  </si>
+  <si>
+    <t>It is common for individuals to encounter barriers or obstacles that make it more difficult for them to change their behavior. For example, a lack of support from one's friends for quitting smoking. Or not having running shoes. When preparing to change one's behavior, it is advantageous to consider potential obstacles to successfully changing one's behavior. To see why, I suggest watching this short video before the next session: https://youtu.be/mdbC9q9pwFw. How do you think can thinking of possible obstacles help you to quit smoking and become more physically active? Collect your thoughts on your phone or a piece of paper.</t>
+  </si>
+  <si>
+    <t>When changing one's behavior, it is possible that in the short term, one's mental and/or physical well-being decline. For example, you may sleep worse for some time after quitting smoking. Such negative effects can make it challenging to both begin and sustain the behavior change. But there are steps that you can take to minimize or even prevent such negative effects. To learn more, I advise watching this short video before the next session: https://youtu.be/3rSqLEgRHEo. What do you think, how can learning about steps to reduce short-term negative effects on your mental and physical well-being help you to quit smoking and become more physically active? Note your thoughts on your phone or a piece of paper.</t>
+  </si>
+  <si>
+    <t>When preparing for becoming more physically active, it can be useful to learn from other people who have succeeded in becoming more physically active. What goal did they set for themselves? And how did they reach it? Before the next session, I thus recommend you watch this short video in which 5 people describe how they reached their physical activity goals: https://youtu.be/m1MHo9fCTG8. What can you take away from the 5 examples for yourself? Take a few notes on a piece of paper or your phone.</t>
   </si>
 </sst>
 </file>
@@ -1990,7 +1990,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2041,12 +2041,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -2080,7 +2074,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2130,9 +2124,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2234,15 +2225,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2251,7 +2242,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2571,54 +2562,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="52"/>
+    <col min="1" max="1" width="9.140625" style="51"/>
     <col min="2" max="2" width="40.42578125" style="8" customWidth="1"/>
-    <col min="3" max="4" width="60.28515625" style="25" customWidth="1"/>
-    <col min="5" max="6" width="60.28515625" style="51" customWidth="1"/>
-    <col min="7" max="7" width="60.28515625" style="56" customWidth="1"/>
-    <col min="8" max="8" width="60.28515625" style="54" customWidth="1"/>
+    <col min="3" max="4" width="60.28515625" style="24" customWidth="1"/>
+    <col min="5" max="6" width="60.28515625" style="50" customWidth="1"/>
+    <col min="7" max="7" width="60.28515625" style="55" customWidth="1"/>
+    <col min="8" max="8" width="60.28515625" style="53" customWidth="1"/>
     <col min="9" max="9" width="60.28515625" style="8" customWidth="1"/>
     <col min="10" max="10" width="50.140625" style="8" customWidth="1"/>
     <col min="11" max="11" width="59.85546875" style="8" customWidth="1"/>
-    <col min="12" max="12" width="57.28515625" style="52" customWidth="1"/>
-    <col min="13" max="13" width="55.28515625" style="25" customWidth="1"/>
+    <col min="12" max="12" width="57.28515625" style="51" customWidth="1"/>
+    <col min="13" max="13" width="55.28515625" style="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="61" t="s">
         <v>129</v>
       </c>
-      <c r="D1" s="62" t="s">
-        <v>256</v>
+      <c r="D1" s="61" t="s">
+        <v>254</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="G1" s="55" t="s">
-        <v>351</v>
-      </c>
-      <c r="H1" s="53" t="s">
-        <v>352</v>
+        <v>212</v>
+      </c>
+      <c r="G1" s="54" t="s">
+        <v>343</v>
+      </c>
+      <c r="H1" s="52" t="s">
+        <v>344</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>130</v>
@@ -2629,12 +2620,12 @@
       <c r="L1" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="M1" s="62" t="s">
-        <v>194</v>
+      <c r="M1" s="61" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="105" x14ac:dyDescent="0.25">
-      <c r="A2" s="52">
+      <c r="A2" s="51">
         <v>0</v>
       </c>
       <c r="B2" s="9" t="s">
@@ -2644,17 +2635,17 @@
         <v>107</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10">
         <v>1</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="I2" s="9"/>
       <c r="J2" s="12"/>
@@ -2667,7 +2658,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="105" x14ac:dyDescent="0.25">
-      <c r="A3" s="52">
+      <c r="A3" s="51">
         <v>1</v>
       </c>
       <c r="B3" s="14" t="s">
@@ -2677,17 +2668,17 @@
         <v>126</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="15">
         <v>0</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I3" s="14"/>
       <c r="J3" s="16"/>
@@ -2700,7 +2691,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="210" x14ac:dyDescent="0.25">
-      <c r="A4" s="52">
+      <c r="A4" s="51">
         <v>2</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -2710,14 +2701,14 @@
         <v>89</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E4" s="10"/>
       <c r="F4" s="10">
         <v>3</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="H4" s="11" t="s">
         <v>177</v>
@@ -2728,14 +2719,14 @@
       </c>
       <c r="K4" s="19"/>
       <c r="L4" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M4" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="150" x14ac:dyDescent="0.25">
-      <c r="A5" s="52">
+      <c r="A5" s="51">
         <v>3</v>
       </c>
       <c r="B5" s="14" t="s">
@@ -2745,30 +2736,30 @@
         <v>112</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="15">
         <v>2</v>
       </c>
-      <c r="G5" s="21" t="s">
-        <v>254</v>
-      </c>
-      <c r="H5" s="21" t="s">
-        <v>178</v>
+      <c r="G5" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>393</v>
       </c>
       <c r="I5" s="14"/>
       <c r="J5" s="16"/>
       <c r="K5" s="16"/>
       <c r="L5" s="14" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="M5" s="14" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="210" x14ac:dyDescent="0.25">
-      <c r="A6" s="52">
+      <c r="A6" s="51">
         <v>4</v>
       </c>
       <c r="B6" s="9" t="s">
@@ -2778,34 +2769,34 @@
         <v>123</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="10" t="s">
-        <v>353</v>
-      </c>
-      <c r="G6" s="22" t="s">
-        <v>224</v>
-      </c>
-      <c r="H6" s="22" t="s">
+        <v>345</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="H6" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="I6" s="23" t="s">
+      <c r="I6" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="J6" s="23" t="s">
+      <c r="J6" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="K6" s="23"/>
+      <c r="K6" s="22"/>
       <c r="L6" s="9" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="210" x14ac:dyDescent="0.25">
-      <c r="A7" s="52">
+      <c r="A7" s="51">
         <v>5</v>
       </c>
       <c r="B7" s="14" t="s">
@@ -2815,34 +2806,34 @@
         <v>124</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="15" t="s">
-        <v>354</v>
-      </c>
-      <c r="G7" s="22" t="s">
-        <v>225</v>
-      </c>
-      <c r="H7" s="22" t="s">
+        <v>346</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="H7" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="I7" s="24" t="s">
+      <c r="I7" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="J7" s="24" t="s">
+      <c r="J7" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="K7" s="24"/>
+      <c r="K7" s="23"/>
       <c r="L7" s="14" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="M7" s="14" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="195" x14ac:dyDescent="0.25">
-      <c r="A8" s="52">
+      <c r="A8" s="51">
         <v>6</v>
       </c>
       <c r="B8" s="9" t="s">
@@ -2852,12 +2843,12 @@
         <v>37</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
       <c r="G8" s="11" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="H8" s="11" t="s">
         <v>137</v>
@@ -2865,21 +2856,21 @@
       <c r="I8" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="J8" s="23" t="s">
+      <c r="J8" s="22" t="s">
         <v>1</v>
       </c>
       <c r="K8" s="13" t="s">
         <v>34</v>
       </c>
       <c r="L8" s="13" t="s">
-        <v>183</v>
-      </c>
-      <c r="M8" s="25" t="s">
-        <v>195</v>
+        <v>181</v>
+      </c>
+      <c r="M8" s="24" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="150" x14ac:dyDescent="0.25">
-      <c r="A9" s="52">
+      <c r="A9" s="51">
         <v>7</v>
       </c>
       <c r="B9" s="14" t="s">
@@ -2889,32 +2880,32 @@
         <v>50</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
-      <c r="G9" s="22" t="s">
-        <v>227</v>
-      </c>
-      <c r="H9" s="22" t="s">
+      <c r="G9" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="H9" s="21" t="s">
         <v>139</v>
       </c>
       <c r="I9" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="J9" s="24" t="s">
+      <c r="J9" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="24"/>
+      <c r="K9" s="23"/>
       <c r="L9" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="M9" s="25" t="s">
-        <v>196</v>
+        <v>182</v>
+      </c>
+      <c r="M9" s="24" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="150" x14ac:dyDescent="0.25">
-      <c r="A10" s="52">
+      <c r="A10" s="51">
         <v>8</v>
       </c>
       <c r="B10" s="9" t="s">
@@ -2924,34 +2915,34 @@
         <v>75</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="10">
         <v>9</v>
       </c>
-      <c r="G10" s="22" t="s">
-        <v>228</v>
-      </c>
-      <c r="H10" s="22" t="s">
+      <c r="G10" s="21" t="s">
+        <v>226</v>
+      </c>
+      <c r="H10" s="21" t="s">
         <v>9</v>
       </c>
       <c r="I10" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="J10" s="23" t="s">
+      <c r="J10" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="K10" s="23"/>
+      <c r="K10" s="22"/>
       <c r="L10" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="M10" s="25" t="s">
-        <v>196</v>
+        <v>182</v>
+      </c>
+      <c r="M10" s="24" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="195" x14ac:dyDescent="0.25">
-      <c r="A11" s="52">
+      <c r="A11" s="51">
         <v>9</v>
       </c>
       <c r="B11" s="14" t="s">
@@ -2961,14 +2952,14 @@
         <v>81</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="15">
         <v>8</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H11" s="11" t="s">
         <v>142</v>
@@ -2976,19 +2967,19 @@
       <c r="I11" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="J11" s="24" t="s">
+      <c r="J11" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="K11" s="24"/>
+      <c r="K11" s="23"/>
       <c r="L11" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="M11" s="25" t="s">
-        <v>196</v>
+        <v>182</v>
+      </c>
+      <c r="M11" s="24" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="225" x14ac:dyDescent="0.25">
-      <c r="A12" s="52">
+      <c r="A12" s="51">
         <v>10</v>
       </c>
       <c r="B12" s="9" t="s">
@@ -2998,19 +2989,19 @@
         <v>104</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="F12" s="10">
         <v>11</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="I12" s="9"/>
       <c r="J12" s="12"/>
@@ -3020,12 +3011,12 @@
       <c r="L12" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="M12" s="25" t="s">
-        <v>197</v>
+      <c r="M12" s="24" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="225" x14ac:dyDescent="0.25">
-      <c r="A13" s="52">
+      <c r="A13" s="51">
         <v>11</v>
       </c>
       <c r="B13" s="14" t="s">
@@ -3035,32 +3026,32 @@
         <v>105</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="F13" s="15">
         <v>10</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="I13" s="14"/>
       <c r="J13" s="16"/>
       <c r="K13" s="17"/>
       <c r="L13" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="M13" s="25" t="s">
-        <v>197</v>
+        <v>207</v>
+      </c>
+      <c r="M13" s="24" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="195" x14ac:dyDescent="0.25">
-      <c r="A14" s="52">
+      <c r="A14" s="51">
         <v>12</v>
       </c>
       <c r="B14" s="9" t="s">
@@ -3070,32 +3061,32 @@
         <v>127</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="10" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="I14" s="9"/>
       <c r="J14" s="12"/>
-      <c r="K14" s="26" t="s">
+      <c r="K14" s="25" t="s">
         <v>113</v>
       </c>
       <c r="L14" s="20" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="M14" s="9" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="180" x14ac:dyDescent="0.25">
-      <c r="A15" s="52">
+      <c r="A15" s="51">
         <v>13</v>
       </c>
       <c r="B15" s="14" t="s">
@@ -3105,100 +3096,100 @@
         <v>60</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E15" s="15"/>
       <c r="F15" s="15" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="I15" s="14"/>
       <c r="J15" s="16"/>
-      <c r="K15" s="27" t="s">
+      <c r="K15" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="L15" s="28" t="s">
-        <v>208</v>
+      <c r="L15" s="27" t="s">
+        <v>206</v>
       </c>
       <c r="M15" s="14" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="225" x14ac:dyDescent="0.25">
-      <c r="A16" s="52">
+      <c r="A16" s="51">
         <v>14</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>108</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>391</v>
+        <v>380</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="10">
         <v>15</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="I16" s="9"/>
       <c r="J16" s="12"/>
       <c r="K16" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="L16" s="29" t="s">
+      <c r="L16" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="M16" s="25" t="s">
-        <v>198</v>
+      <c r="M16" s="24" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="135" x14ac:dyDescent="0.25">
-      <c r="A17" s="52">
+      <c r="A17" s="51">
         <v>15</v>
       </c>
       <c r="B17" s="14" t="s">
         <v>114</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>392</v>
+        <v>381</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E17" s="15"/>
       <c r="F17" s="15">
         <v>14</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="I17" s="14"/>
       <c r="J17" s="16"/>
       <c r="K17" s="16"/>
-      <c r="L17" s="30" t="s">
+      <c r="L17" s="29" t="s">
         <v>176</v>
       </c>
-      <c r="M17" s="25" t="s">
-        <v>198</v>
+      <c r="M17" s="24" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="150" x14ac:dyDescent="0.25">
-      <c r="A18" s="52">
+      <c r="A18" s="51">
         <v>16</v>
       </c>
       <c r="B18" s="9" t="s">
@@ -3208,12 +3199,12 @@
         <v>77</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="11" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="H18" s="11" t="s">
         <v>11</v>
@@ -3221,19 +3212,19 @@
       <c r="I18" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="J18" s="23" t="s">
+      <c r="J18" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="K18" s="23"/>
+      <c r="K18" s="22"/>
       <c r="L18" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="M18" s="25" t="s">
-        <v>199</v>
+        <v>183</v>
+      </c>
+      <c r="M18" s="24" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="210" x14ac:dyDescent="0.25">
-      <c r="A19" s="52">
+      <c r="A19" s="51">
         <v>17</v>
       </c>
       <c r="B19" s="14" t="s">
@@ -3243,12 +3234,12 @@
         <v>78</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
       <c r="G19" s="11" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H19" s="11" t="s">
         <v>143</v>
@@ -3256,19 +3247,19 @@
       <c r="I19" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="J19" s="24" t="s">
+      <c r="J19" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="K19" s="24"/>
+      <c r="K19" s="23"/>
       <c r="L19" s="14" t="s">
-        <v>185</v>
-      </c>
-      <c r="M19" s="25" t="s">
-        <v>199</v>
+        <v>183</v>
+      </c>
+      <c r="M19" s="24" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="150" x14ac:dyDescent="0.25">
-      <c r="A20" s="52">
+      <c r="A20" s="51">
         <v>18</v>
       </c>
       <c r="B20" s="9" t="s">
@@ -3278,14 +3269,14 @@
         <v>118</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="10" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H20" s="11" t="s">
         <v>145</v>
@@ -3293,19 +3284,19 @@
       <c r="I20" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="J20" s="23" t="s">
+      <c r="J20" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="K20" s="23"/>
+      <c r="K20" s="22"/>
       <c r="L20" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="M20" s="25" t="s">
-        <v>199</v>
+        <v>182</v>
+      </c>
+      <c r="M20" s="24" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="210" x14ac:dyDescent="0.25">
-      <c r="A21" s="52">
+      <c r="A21" s="51">
         <v>19</v>
       </c>
       <c r="B21" s="14" t="s">
@@ -3315,14 +3306,14 @@
         <v>117</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E21" s="15"/>
       <c r="F21" s="15" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="H21" s="11" t="s">
         <v>147</v>
@@ -3330,19 +3321,19 @@
       <c r="I21" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="J21" s="24" t="s">
+      <c r="J21" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="K21" s="24"/>
+      <c r="K21" s="23"/>
       <c r="L21" s="14" t="s">
-        <v>186</v>
-      </c>
-      <c r="M21" s="25" t="s">
-        <v>200</v>
+        <v>184</v>
+      </c>
+      <c r="M21" s="24" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="210" x14ac:dyDescent="0.25">
-      <c r="A22" s="52">
+      <c r="A22" s="51">
         <v>20</v>
       </c>
       <c r="B22" s="9" t="s">
@@ -3352,14 +3343,14 @@
         <v>120</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="10" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="H22" s="11" t="s">
         <v>148</v>
@@ -3367,19 +3358,19 @@
       <c r="I22" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="J22" s="23" t="s">
+      <c r="J22" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="K22" s="23"/>
+      <c r="K22" s="22"/>
       <c r="L22" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="M22" s="25" t="s">
-        <v>200</v>
+        <v>184</v>
+      </c>
+      <c r="M22" s="24" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="225" x14ac:dyDescent="0.25">
-      <c r="A23" s="52">
+      <c r="A23" s="51">
         <v>21</v>
       </c>
       <c r="B23" s="14" t="s">
@@ -3389,14 +3380,14 @@
         <v>119</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E23" s="15"/>
       <c r="F23" s="15" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="H23" s="11" t="s">
         <v>150</v>
@@ -3404,19 +3395,19 @@
       <c r="I23" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="J23" s="24" t="s">
+      <c r="J23" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="K23" s="24"/>
+      <c r="K23" s="23"/>
       <c r="L23" s="14" t="s">
-        <v>186</v>
-      </c>
-      <c r="M23" s="25" t="s">
-        <v>200</v>
+        <v>184</v>
+      </c>
+      <c r="M23" s="24" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="150" x14ac:dyDescent="0.25">
-      <c r="A24" s="52">
+      <c r="A24" s="51">
         <v>22</v>
       </c>
       <c r="B24" s="9" t="s">
@@ -3426,14 +3417,14 @@
         <v>109</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E24" s="10"/>
       <c r="F24" s="10">
         <v>23</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H24" s="11" t="s">
         <v>151</v>
@@ -3441,19 +3432,19 @@
       <c r="I24" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="J24" s="23" t="s">
+      <c r="J24" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="K24" s="23"/>
+      <c r="K24" s="22"/>
       <c r="L24" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="M24" s="25" t="s">
-        <v>199</v>
+        <v>182</v>
+      </c>
+      <c r="M24" s="24" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="180" x14ac:dyDescent="0.25">
-      <c r="A25" s="52">
+      <c r="A25" s="51">
         <v>23</v>
       </c>
       <c r="B25" s="14" t="s">
@@ -3463,14 +3454,14 @@
         <v>92</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E25" s="15"/>
       <c r="F25" s="15">
         <v>22</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="H25" s="11" t="s">
         <v>153</v>
@@ -3478,19 +3469,19 @@
       <c r="I25" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="J25" s="24" t="s">
+      <c r="J25" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="K25" s="24"/>
+      <c r="K25" s="23"/>
       <c r="L25" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="M25" s="25" t="s">
-        <v>199</v>
+        <v>182</v>
+      </c>
+      <c r="M25" s="24" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="210" x14ac:dyDescent="0.25">
-      <c r="A26" s="52">
+      <c r="A26" s="51">
         <v>24</v>
       </c>
       <c r="B26" s="9" t="s">
@@ -3500,17 +3491,17 @@
         <v>121</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E26" s="10"/>
       <c r="F26" s="10" t="s">
-        <v>361</v>
-      </c>
-      <c r="G26" s="22" t="s">
-        <v>376</v>
-      </c>
-      <c r="H26" s="22" t="s">
-        <v>377</v>
+        <v>353</v>
+      </c>
+      <c r="G26" s="21" t="s">
+        <v>368</v>
+      </c>
+      <c r="H26" s="21" t="s">
+        <v>369</v>
       </c>
       <c r="I26" s="9" t="s">
         <v>166</v>
@@ -3518,14 +3509,14 @@
       <c r="J26" s="12"/>
       <c r="K26" s="12"/>
       <c r="L26" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="M26" s="25" t="s">
-        <v>200</v>
+        <v>184</v>
+      </c>
+      <c r="M26" s="24" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="210" x14ac:dyDescent="0.25">
-      <c r="A27" s="52">
+      <c r="A27" s="51">
         <v>25</v>
       </c>
       <c r="B27" s="14" t="s">
@@ -3535,14 +3526,14 @@
         <v>122</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E27" s="15"/>
       <c r="F27" s="15" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H27" s="11" t="s">
         <v>154</v>
@@ -3550,910 +3541,910 @@
       <c r="I27" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="J27" s="24" t="s">
+      <c r="J27" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="K27" s="24"/>
+      <c r="K27" s="23"/>
       <c r="L27" s="14" t="s">
-        <v>186</v>
-      </c>
-      <c r="M27" s="25" t="s">
-        <v>200</v>
+        <v>184</v>
+      </c>
+      <c r="M27" s="24" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="225" x14ac:dyDescent="0.25">
-      <c r="A28" s="52">
+      <c r="A28" s="51">
         <v>26</v>
       </c>
-      <c r="B28" s="31" t="s">
+      <c r="B28" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="31" t="s">
+      <c r="C28" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="D28" s="31" t="s">
+      <c r="D28" s="30" t="s">
+        <v>280</v>
+      </c>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="11" t="s">
+        <v>370</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>371</v>
+      </c>
+      <c r="I28" s="30"/>
+      <c r="J28" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="K28" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="L28" s="33" t="s">
+        <v>167</v>
+      </c>
+      <c r="M28" s="24" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="135" x14ac:dyDescent="0.25">
+      <c r="A29" s="51">
+        <v>27</v>
+      </c>
+      <c r="B29" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" s="30" t="s">
+        <v>281</v>
+      </c>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="11" t="s">
+        <v>372</v>
+      </c>
+      <c r="H29" s="11" t="s">
+        <v>373</v>
+      </c>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="K29" s="34"/>
+      <c r="L29" s="30" t="s">
+        <v>168</v>
+      </c>
+      <c r="M29" s="30" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="180" x14ac:dyDescent="0.25">
+      <c r="A30" s="51">
+        <v>28</v>
+      </c>
+      <c r="B30" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" s="30" t="s">
         <v>282</v>
       </c>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="11" t="s">
-        <v>378</v>
-      </c>
-      <c r="H28" s="11" t="s">
-        <v>379</v>
-      </c>
-      <c r="I28" s="31"/>
-      <c r="J28" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="K28" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="L28" s="34" t="s">
-        <v>167</v>
-      </c>
-      <c r="M28" s="25" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="135" x14ac:dyDescent="0.25">
-      <c r="A29" s="52">
-        <v>27</v>
-      </c>
-      <c r="B29" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="C29" s="31" t="s">
-        <v>88</v>
-      </c>
-      <c r="D29" s="31" t="s">
+      <c r="E30" s="31">
+        <v>16</v>
+      </c>
+      <c r="F30" s="31"/>
+      <c r="G30" s="21" t="s">
+        <v>238</v>
+      </c>
+      <c r="H30" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="I30" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="J30" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="K30" s="35"/>
+      <c r="L30" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="M30" s="24" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="150" x14ac:dyDescent="0.25">
+      <c r="A31" s="51">
+        <v>29</v>
+      </c>
+      <c r="B31" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" s="30" t="s">
         <v>283</v>
       </c>
-      <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="11" t="s">
-        <v>380</v>
-      </c>
-      <c r="H29" s="11" t="s">
-        <v>381</v>
-      </c>
-      <c r="I29" s="31"/>
-      <c r="J29" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="K29" s="35"/>
-      <c r="L29" s="31" t="s">
-        <v>168</v>
-      </c>
-      <c r="M29" s="31" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="180" x14ac:dyDescent="0.25">
-      <c r="A30" s="52">
-        <v>28</v>
-      </c>
-      <c r="B30" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="C30" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="D30" s="31" t="s">
-        <v>284</v>
-      </c>
-      <c r="E30" s="32">
+      <c r="E31" s="31">
         <v>16</v>
       </c>
-      <c r="F30" s="32"/>
-      <c r="G30" s="22" t="s">
-        <v>240</v>
-      </c>
-      <c r="H30" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="I30" s="31" t="s">
-        <v>141</v>
-      </c>
-      <c r="J30" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="K30" s="36"/>
-      <c r="L30" s="31" t="s">
-        <v>187</v>
-      </c>
-      <c r="M30" s="25" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="150" x14ac:dyDescent="0.25">
-      <c r="A31" s="52">
-        <v>29</v>
-      </c>
-      <c r="B31" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="C31" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="D31" s="31" t="s">
-        <v>285</v>
-      </c>
-      <c r="E31" s="32">
-        <v>16</v>
-      </c>
-      <c r="F31" s="32"/>
+      <c r="F31" s="31"/>
       <c r="G31" s="11" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="H31" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="I31" s="31" t="s">
+      <c r="I31" s="30" t="s">
         <v>152</v>
       </c>
-      <c r="J31" s="36" t="s">
+      <c r="J31" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="K31" s="36"/>
-      <c r="L31" s="31" t="s">
-        <v>184</v>
-      </c>
-      <c r="M31" s="25" t="s">
-        <v>199</v>
+      <c r="K31" s="35"/>
+      <c r="L31" s="30" t="s">
+        <v>182</v>
+      </c>
+      <c r="M31" s="24" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="165" x14ac:dyDescent="0.25">
-      <c r="A32" s="52">
+      <c r="A32" s="51">
         <v>30</v>
       </c>
-      <c r="B32" s="31" t="s">
+      <c r="B32" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="C32" s="31" t="s">
+      <c r="C32" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="D32" s="31" t="s">
-        <v>286</v>
-      </c>
-      <c r="E32" s="32"/>
-      <c r="F32" s="32"/>
-      <c r="G32" s="22" t="s">
-        <v>242</v>
-      </c>
-      <c r="H32" s="22" t="s">
+      <c r="D32" s="30" t="s">
+        <v>284</v>
+      </c>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="H32" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="I32" s="31" t="s">
+      <c r="I32" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="J32" s="36" t="s">
+      <c r="J32" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="K32" s="37" t="s">
+      <c r="K32" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="L32" s="37" t="s">
-        <v>184</v>
-      </c>
-      <c r="M32" s="25" t="s">
-        <v>199</v>
+      <c r="L32" s="36" t="s">
+        <v>182</v>
+      </c>
+      <c r="M32" s="24" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="165" x14ac:dyDescent="0.25">
-      <c r="A33" s="52">
+      <c r="A33" s="51">
         <v>31</v>
       </c>
-      <c r="B33" s="31" t="s">
+      <c r="B33" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="31" t="s">
+      <c r="C33" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="D33" s="31" t="s">
-        <v>287</v>
-      </c>
-      <c r="E33" s="32"/>
-      <c r="F33" s="32">
+      <c r="D33" s="30" t="s">
+        <v>285</v>
+      </c>
+      <c r="E33" s="31"/>
+      <c r="F33" s="31">
         <v>32</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H33" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="I33" s="31" t="s">
+      <c r="I33" s="30" t="s">
         <v>158</v>
       </c>
-      <c r="J33" s="36" t="s">
+      <c r="J33" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="K33" s="36"/>
-      <c r="L33" s="31" t="s">
-        <v>184</v>
-      </c>
-      <c r="M33" s="25" t="s">
-        <v>199</v>
+      <c r="K33" s="35"/>
+      <c r="L33" s="30" t="s">
+        <v>182</v>
+      </c>
+      <c r="M33" s="24" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="135" x14ac:dyDescent="0.25">
-      <c r="A34" s="52">
+      <c r="A34" s="51">
         <v>32</v>
       </c>
-      <c r="B34" s="31" t="s">
+      <c r="B34" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="C34" s="31" t="s">
+      <c r="C34" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="D34" s="31" t="s">
-        <v>288</v>
-      </c>
-      <c r="E34" s="32"/>
-      <c r="F34" s="32">
+      <c r="D34" s="30" t="s">
+        <v>286</v>
+      </c>
+      <c r="E34" s="31"/>
+      <c r="F34" s="31">
         <v>31</v>
       </c>
       <c r="G34" s="11" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="H34" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="I34" s="31"/>
-      <c r="J34" s="38" t="s">
+      <c r="I34" s="30"/>
+      <c r="J34" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="K34" s="33"/>
-      <c r="L34" s="39" t="s">
+      <c r="K34" s="32"/>
+      <c r="L34" s="38" t="s">
         <v>169</v>
       </c>
-      <c r="M34" s="39" t="s">
+      <c r="M34" s="38" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="180" x14ac:dyDescent="0.25">
-      <c r="A35" s="52">
+      <c r="A35" s="51">
         <v>33</v>
       </c>
-      <c r="B35" s="31" t="s">
+      <c r="B35" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="C35" s="31" t="s">
+      <c r="C35" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="D35" s="31" t="s">
+      <c r="D35" s="30" t="s">
+        <v>287</v>
+      </c>
+      <c r="E35" s="31">
+        <v>34</v>
+      </c>
+      <c r="F35" s="31"/>
+      <c r="G35" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="H35" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="I35" s="30"/>
+      <c r="J35" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="K35" s="32"/>
+      <c r="L35" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="M35" s="38" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="180" x14ac:dyDescent="0.25">
+      <c r="A36" s="51">
+        <v>34</v>
+      </c>
+      <c r="B36" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="C36" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="D36" s="30" t="s">
+        <v>288</v>
+      </c>
+      <c r="E36" s="31"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="I36" s="30"/>
+      <c r="J36" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="K36" s="32"/>
+      <c r="L36" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="M36" s="38" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="150" x14ac:dyDescent="0.25">
+      <c r="A37" s="51">
+        <v>35</v>
+      </c>
+      <c r="B37" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="C37" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="D37" s="30" t="s">
         <v>289</v>
       </c>
-      <c r="E35" s="32">
-        <v>34</v>
-      </c>
-      <c r="F35" s="32"/>
-      <c r="G35" s="11" t="s">
-        <v>251</v>
-      </c>
-      <c r="H35" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="I35" s="31"/>
-      <c r="J35" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="K35" s="33"/>
-      <c r="L35" s="35" t="s">
-        <v>171</v>
-      </c>
-      <c r="M35" s="39" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" ht="180" x14ac:dyDescent="0.25">
-      <c r="A36" s="52">
-        <v>34</v>
-      </c>
-      <c r="B36" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="C36" s="31" t="s">
-        <v>85</v>
-      </c>
-      <c r="D36" s="31" t="s">
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
+      <c r="G37" s="11" t="s">
+        <v>374</v>
+      </c>
+      <c r="H37" s="11" t="s">
+        <v>383</v>
+      </c>
+      <c r="I37" s="30"/>
+      <c r="J37" s="37" t="s">
+        <v>172</v>
+      </c>
+      <c r="K37" s="32"/>
+      <c r="L37" s="39" t="s">
+        <v>173</v>
+      </c>
+      <c r="M37" s="39" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="150" x14ac:dyDescent="0.25">
+      <c r="A38" s="51">
+        <v>36</v>
+      </c>
+      <c r="B38" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="C38" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="D38" s="30" t="s">
         <v>290</v>
       </c>
-      <c r="E36" s="32"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="11" t="s">
-        <v>248</v>
-      </c>
-      <c r="H36" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="I36" s="31"/>
-      <c r="J36" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="K36" s="33"/>
-      <c r="L36" s="35" t="s">
-        <v>171</v>
-      </c>
-      <c r="M36" s="39" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" ht="150" x14ac:dyDescent="0.25">
-      <c r="A37" s="52">
-        <v>35</v>
-      </c>
-      <c r="B37" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="C37" s="31" t="s">
-        <v>87</v>
-      </c>
-      <c r="D37" s="31" t="s">
-        <v>291</v>
-      </c>
-      <c r="E37" s="32"/>
-      <c r="F37" s="32"/>
-      <c r="G37" s="21" t="s">
-        <v>382</v>
-      </c>
-      <c r="H37" s="21" t="s">
-        <v>383</v>
-      </c>
-      <c r="I37" s="31"/>
-      <c r="J37" s="38" t="s">
-        <v>172</v>
-      </c>
-      <c r="K37" s="33"/>
-      <c r="L37" s="40" t="s">
-        <v>173</v>
-      </c>
-      <c r="M37" s="40" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" ht="150" x14ac:dyDescent="0.25">
-      <c r="A38" s="52">
-        <v>36</v>
-      </c>
-      <c r="B38" s="31" t="s">
-        <v>90</v>
-      </c>
-      <c r="C38" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="D38" s="31" t="s">
-        <v>292</v>
-      </c>
-      <c r="E38" s="32"/>
-      <c r="F38" s="32"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="31"/>
       <c r="G38" s="11" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="H38" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="I38" s="31" t="s">
+      <c r="I38" s="30" t="s">
         <v>152</v>
       </c>
-      <c r="J38" s="36" t="s">
+      <c r="J38" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="K38" s="36"/>
-      <c r="L38" s="31" t="s">
-        <v>184</v>
-      </c>
-      <c r="M38" s="25" t="s">
-        <v>199</v>
+      <c r="K38" s="35"/>
+      <c r="L38" s="30" t="s">
+        <v>182</v>
+      </c>
+      <c r="M38" s="24" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="180" x14ac:dyDescent="0.25">
-      <c r="A39" s="52">
+      <c r="A39" s="51">
         <v>37</v>
       </c>
-      <c r="B39" s="41" t="s">
+      <c r="B39" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="C39" s="41" t="s">
+      <c r="C39" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="D39" s="41" t="s">
-        <v>293</v>
-      </c>
-      <c r="E39" s="42"/>
-      <c r="F39" s="42"/>
+      <c r="D39" s="40" t="s">
+        <v>291</v>
+      </c>
+      <c r="E39" s="41"/>
+      <c r="F39" s="41"/>
       <c r="G39" s="11" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="H39" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="I39" s="41"/>
-      <c r="J39" s="43"/>
-      <c r="K39" s="41" t="s">
+      <c r="I39" s="40"/>
+      <c r="J39" s="42"/>
+      <c r="K39" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="L39" s="44" t="s">
+      <c r="L39" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="M39" s="25" t="s">
+      <c r="M39" s="24" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="180" x14ac:dyDescent="0.25">
+      <c r="A40" s="51">
+        <v>38</v>
+      </c>
+      <c r="B40" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="C40" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="D40" s="40" t="s">
+        <v>292</v>
+      </c>
+      <c r="E40" s="41"/>
+      <c r="F40" s="41"/>
+      <c r="G40" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="H40" s="11" t="s">
+        <v>384</v>
+      </c>
+      <c r="I40" s="40" t="s">
+        <v>200</v>
+      </c>
+      <c r="J40" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="K40" s="44" t="s">
+        <v>71</v>
+      </c>
+      <c r="L40" s="40" t="s">
+        <v>186</v>
+      </c>
+      <c r="M40" s="24" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="180" x14ac:dyDescent="0.25">
-      <c r="A40" s="52">
-        <v>38</v>
-      </c>
-      <c r="B40" s="41" t="s">
-        <v>93</v>
-      </c>
-      <c r="C40" s="41" t="s">
-        <v>57</v>
-      </c>
-      <c r="D40" s="41" t="s">
-        <v>294</v>
-      </c>
-      <c r="E40" s="42"/>
-      <c r="F40" s="42"/>
-      <c r="G40" s="21" t="s">
-        <v>255</v>
-      </c>
-      <c r="H40" s="21" t="s">
-        <v>180</v>
-      </c>
-      <c r="I40" s="41" t="s">
-        <v>202</v>
-      </c>
-      <c r="J40" s="45" t="s">
-        <v>22</v>
-      </c>
-      <c r="K40" s="45" t="s">
-        <v>71</v>
-      </c>
-      <c r="L40" s="41" t="s">
-        <v>188</v>
-      </c>
-      <c r="M40" s="25" t="s">
-        <v>203</v>
-      </c>
-    </row>
     <row r="41" spans="1:13" ht="390" x14ac:dyDescent="0.25">
-      <c r="A41" s="52">
+      <c r="A41" s="51">
         <v>39</v>
       </c>
-      <c r="B41" s="41" t="s">
+      <c r="B41" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="C41" s="41" t="s">
+      <c r="C41" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="D41" s="41" t="s">
-        <v>295</v>
-      </c>
-      <c r="E41" s="42"/>
-      <c r="F41" s="42"/>
+      <c r="D41" s="40" t="s">
+        <v>293</v>
+      </c>
+      <c r="E41" s="41"/>
+      <c r="F41" s="41"/>
       <c r="G41" s="11" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H41" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="I41" s="41" t="s">
+      <c r="I41" s="40" t="s">
         <v>155</v>
       </c>
-      <c r="J41" s="41" t="s">
+      <c r="J41" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="K41" s="45" t="s">
+      <c r="K41" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="L41" s="41" t="s">
-        <v>189</v>
-      </c>
-      <c r="M41" s="25" t="s">
-        <v>204</v>
+      <c r="L41" s="40" t="s">
+        <v>187</v>
+      </c>
+      <c r="M41" s="24" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="210" x14ac:dyDescent="0.25">
-      <c r="A42" s="52">
+      <c r="A42" s="51">
         <v>40</v>
       </c>
-      <c r="B42" s="41" t="s">
+      <c r="B42" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="C42" s="41" t="s">
+      <c r="C42" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="D42" s="41" t="s">
-        <v>296</v>
-      </c>
-      <c r="E42" s="42">
+      <c r="D42" s="40" t="s">
+        <v>294</v>
+      </c>
+      <c r="E42" s="41">
         <v>17</v>
       </c>
-      <c r="F42" s="42"/>
+      <c r="F42" s="41"/>
       <c r="G42" s="11" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="H42" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="I42" s="41" t="s">
+      <c r="I42" s="40" t="s">
         <v>155</v>
       </c>
-      <c r="J42" s="45" t="s">
+      <c r="J42" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="K42" s="45"/>
-      <c r="L42" s="41" t="s">
-        <v>190</v>
-      </c>
-      <c r="M42" s="25" t="s">
-        <v>205</v>
+      <c r="K42" s="44"/>
+      <c r="L42" s="40" t="s">
+        <v>188</v>
+      </c>
+      <c r="M42" s="24" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="165" x14ac:dyDescent="0.25">
-      <c r="A43" s="52">
+      <c r="A43" s="51">
         <v>41</v>
       </c>
-      <c r="B43" s="41" t="s">
+      <c r="B43" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="C43" s="41" t="s">
+      <c r="C43" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="D43" s="41" t="s">
-        <v>297</v>
-      </c>
-      <c r="E43" s="42">
+      <c r="D43" s="40" t="s">
+        <v>295</v>
+      </c>
+      <c r="E43" s="41">
         <v>17</v>
       </c>
-      <c r="F43" s="42"/>
+      <c r="F43" s="41"/>
       <c r="G43" s="11" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="H43" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="I43" s="41" t="s">
+      <c r="I43" s="40" t="s">
         <v>155</v>
       </c>
-      <c r="J43" s="45" t="s">
+      <c r="J43" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="K43" s="45"/>
-      <c r="L43" s="41" t="s">
-        <v>190</v>
-      </c>
-      <c r="M43" s="25" t="s">
+      <c r="K43" s="44"/>
+      <c r="L43" s="40" t="s">
+        <v>188</v>
+      </c>
+      <c r="M43" s="24" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" s="1" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A44" s="51">
+        <v>42</v>
+      </c>
+      <c r="B44" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="C44" s="45" t="s">
+        <v>125</v>
+      </c>
+      <c r="D44" s="45" t="s">
+        <v>296</v>
+      </c>
+      <c r="E44" s="46"/>
+      <c r="F44" s="46"/>
+      <c r="G44" s="11" t="s">
+        <v>375</v>
+      </c>
+      <c r="H44" s="11" t="s">
+        <v>375</v>
+      </c>
+      <c r="I44" s="45"/>
+      <c r="J44" s="47"/>
+      <c r="K44" s="47"/>
+      <c r="L44" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="M44" s="45" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" s="1" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A45" s="51">
+        <v>43</v>
+      </c>
+      <c r="B45" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="C45" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="D45" s="45" t="s">
+        <v>299</v>
+      </c>
+      <c r="E45" s="46"/>
+      <c r="F45" s="46" t="s">
+        <v>355</v>
+      </c>
+      <c r="G45" s="11" t="s">
+        <v>376</v>
+      </c>
+      <c r="H45" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="I45" s="45"/>
+      <c r="J45" s="47"/>
+      <c r="K45" s="49" t="s">
+        <v>29</v>
+      </c>
+      <c r="L45" s="48" t="s">
+        <v>165</v>
+      </c>
+      <c r="M45" s="45" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="44" spans="1:13" s="1" customFormat="1" ht="180" x14ac:dyDescent="0.25">
-      <c r="A44" s="52">
-        <v>42</v>
-      </c>
-      <c r="B44" s="46" t="s">
-        <v>70</v>
-      </c>
-      <c r="C44" s="46" t="s">
-        <v>125</v>
-      </c>
-      <c r="D44" s="46" t="s">
-        <v>298</v>
-      </c>
-      <c r="E44" s="47"/>
-      <c r="F44" s="47"/>
-      <c r="G44" s="11" t="s">
-        <v>384</v>
-      </c>
-      <c r="H44" s="11" t="s">
-        <v>384</v>
-      </c>
-      <c r="I44" s="46"/>
-      <c r="J44" s="48"/>
-      <c r="K44" s="48"/>
-      <c r="L44" s="49" t="s">
-        <v>164</v>
-      </c>
-      <c r="M44" s="46" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" s="1" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="52">
-        <v>43</v>
-      </c>
-      <c r="B45" s="46" t="s">
-        <v>95</v>
-      </c>
-      <c r="C45" s="46" t="s">
-        <v>116</v>
-      </c>
-      <c r="D45" s="46" t="s">
+    <row r="46" spans="1:13" s="59" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A46" s="56">
+        <v>44</v>
+      </c>
+      <c r="B46" s="56" t="s">
+        <v>300</v>
+      </c>
+      <c r="C46" s="60" t="s">
+        <v>315</v>
+      </c>
+      <c r="D46" s="60" t="s">
+        <v>316</v>
+      </c>
+      <c r="E46" s="58"/>
+      <c r="F46" s="58"/>
+      <c r="G46" s="62" t="s">
+        <v>326</v>
+      </c>
+      <c r="H46" s="62" t="s">
+        <v>325</v>
+      </c>
+      <c r="I46" s="57"/>
+      <c r="J46" s="57"/>
+      <c r="K46" s="57"/>
+      <c r="L46" s="56"/>
+      <c r="M46" s="60" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" s="59" customFormat="1" ht="225" x14ac:dyDescent="0.25">
+      <c r="A47" s="56">
+        <v>45</v>
+      </c>
+      <c r="B47" s="56" t="s">
         <v>301</v>
       </c>
-      <c r="E45" s="47"/>
-      <c r="F45" s="47" t="s">
-        <v>363</v>
-      </c>
-      <c r="G45" s="11" t="s">
+      <c r="C47" s="60" t="s">
+        <v>309</v>
+      </c>
+      <c r="D47" s="60" t="s">
+        <v>310</v>
+      </c>
+      <c r="E47" s="58"/>
+      <c r="F47" s="58"/>
+      <c r="G47" s="62" t="s">
+        <v>327</v>
+      </c>
+      <c r="H47" s="62" t="s">
         <v>385</v>
       </c>
-      <c r="H45" s="11" t="s">
+      <c r="I47" s="57"/>
+      <c r="J47" s="57"/>
+      <c r="K47" s="57"/>
+      <c r="L47" s="56"/>
+      <c r="M47" s="60" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" s="59" customFormat="1" ht="270" x14ac:dyDescent="0.25">
+      <c r="A48" s="56">
+        <v>46</v>
+      </c>
+      <c r="B48" s="56" t="s">
+        <v>302</v>
+      </c>
+      <c r="C48" s="60" t="s">
+        <v>311</v>
+      </c>
+      <c r="D48" s="60" t="s">
+        <v>312</v>
+      </c>
+      <c r="E48" s="58"/>
+      <c r="F48" s="58"/>
+      <c r="G48" s="62" t="s">
+        <v>328</v>
+      </c>
+      <c r="H48" s="62" t="s">
         <v>386</v>
       </c>
-      <c r="I45" s="46"/>
-      <c r="J45" s="48"/>
-      <c r="K45" s="50" t="s">
-        <v>29</v>
-      </c>
-      <c r="L45" s="49" t="s">
-        <v>165</v>
-      </c>
-      <c r="M45" s="46" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" s="60" customFormat="1" ht="180" x14ac:dyDescent="0.25">
-      <c r="A46" s="57">
-        <v>44</v>
-      </c>
-      <c r="B46" s="57" t="s">
-        <v>302</v>
-      </c>
-      <c r="C46" s="61" t="s">
+      <c r="I48" s="57"/>
+      <c r="J48" s="57"/>
+      <c r="K48" s="57"/>
+      <c r="L48" s="56"/>
+      <c r="M48" s="60" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" s="59" customFormat="1" ht="255" x14ac:dyDescent="0.25">
+      <c r="A49" s="56">
+        <v>47</v>
+      </c>
+      <c r="B49" s="56" t="s">
+        <v>303</v>
+      </c>
+      <c r="C49" s="60" t="s">
+        <v>313</v>
+      </c>
+      <c r="D49" s="60" t="s">
+        <v>314</v>
+      </c>
+      <c r="E49" s="58"/>
+      <c r="F49" s="58"/>
+      <c r="G49" s="62" t="s">
+        <v>329</v>
+      </c>
+      <c r="H49" s="62" t="s">
+        <v>387</v>
+      </c>
+      <c r="I49" s="57"/>
+      <c r="J49" s="57"/>
+      <c r="K49" s="57"/>
+      <c r="L49" s="56"/>
+      <c r="M49" s="60" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" s="59" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A50" s="56">
+        <v>48</v>
+      </c>
+      <c r="B50" s="56" t="s">
+        <v>304</v>
+      </c>
+      <c r="C50" s="60" t="s">
         <v>317</v>
       </c>
-      <c r="D46" s="61" t="s">
+      <c r="D50" s="60" t="s">
+        <v>324</v>
+      </c>
+      <c r="E50" s="58"/>
+      <c r="F50" s="58"/>
+      <c r="G50" s="62" t="s">
+        <v>330</v>
+      </c>
+      <c r="H50" s="62" t="s">
+        <v>388</v>
+      </c>
+      <c r="I50" s="57"/>
+      <c r="J50" s="57"/>
+      <c r="K50" s="57"/>
+      <c r="L50" s="56"/>
+      <c r="M50" s="63" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" s="59" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A51" s="56">
+        <v>49</v>
+      </c>
+      <c r="B51" s="56" t="s">
+        <v>305</v>
+      </c>
+      <c r="C51" s="60" t="s">
         <v>318</v>
       </c>
-      <c r="E46" s="59"/>
-      <c r="F46" s="59"/>
-      <c r="G46" s="63" t="s">
+      <c r="D51" s="60" t="s">
+        <v>319</v>
+      </c>
+      <c r="E51" s="58"/>
+      <c r="F51" s="58"/>
+      <c r="G51" s="62" t="s">
+        <v>331</v>
+      </c>
+      <c r="H51" s="62" t="s">
+        <v>389</v>
+      </c>
+      <c r="I51" s="57"/>
+      <c r="J51" s="57"/>
+      <c r="K51" s="57"/>
+      <c r="L51" s="56"/>
+      <c r="M51" s="60" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" s="59" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A52" s="56">
+        <v>60</v>
+      </c>
+      <c r="B52" s="56" t="s">
+        <v>306</v>
+      </c>
+      <c r="C52" s="60" t="s">
+        <v>321</v>
+      </c>
+      <c r="D52" s="60" t="s">
+        <v>320</v>
+      </c>
+      <c r="E52" s="58"/>
+      <c r="F52" s="58"/>
+      <c r="G52" s="62" t="s">
+        <v>332</v>
+      </c>
+      <c r="H52" s="62" t="s">
+        <v>390</v>
+      </c>
+      <c r="I52" s="57"/>
+      <c r="J52" s="57"/>
+      <c r="K52" s="57"/>
+      <c r="L52" s="56"/>
+      <c r="M52" s="60" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" s="59" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A53" s="56">
+        <v>51</v>
+      </c>
+      <c r="B53" s="56" t="s">
+        <v>308</v>
+      </c>
+      <c r="C53" s="60" t="s">
+        <v>341</v>
+      </c>
+      <c r="D53" s="60" t="s">
+        <v>342</v>
+      </c>
+      <c r="E53" s="58"/>
+      <c r="F53" s="58"/>
+      <c r="G53" s="62" t="s">
+        <v>378</v>
+      </c>
+      <c r="H53" s="62" t="s">
+        <v>391</v>
+      </c>
+      <c r="I53" s="57"/>
+      <c r="J53" s="57"/>
+      <c r="K53" s="57"/>
+      <c r="L53" s="56"/>
+      <c r="M53" s="63" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" s="59" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A54" s="56">
+        <v>52</v>
+      </c>
+      <c r="B54" s="56" t="s">
+        <v>307</v>
+      </c>
+      <c r="C54" s="60" t="s">
+        <v>322</v>
+      </c>
+      <c r="D54" s="60" t="s">
+        <v>323</v>
+      </c>
+      <c r="E54" s="58"/>
+      <c r="F54" s="58"/>
+      <c r="G54" s="62" t="s">
+        <v>379</v>
+      </c>
+      <c r="H54" s="62" t="s">
+        <v>392</v>
+      </c>
+      <c r="I54" s="57"/>
+      <c r="J54" s="57"/>
+      <c r="K54" s="57"/>
+      <c r="L54" s="56"/>
+      <c r="M54" s="60" t="s">
         <v>334</v>
-      </c>
-      <c r="H46" s="63" t="s">
-        <v>327</v>
-      </c>
-      <c r="I46" s="58"/>
-      <c r="J46" s="58"/>
-      <c r="K46" s="58"/>
-      <c r="L46" s="57"/>
-      <c r="M46" s="61" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" s="60" customFormat="1" ht="225" x14ac:dyDescent="0.25">
-      <c r="A47" s="57">
-        <v>45</v>
-      </c>
-      <c r="B47" s="57" t="s">
-        <v>303</v>
-      </c>
-      <c r="C47" s="61" t="s">
-        <v>311</v>
-      </c>
-      <c r="D47" s="61" t="s">
-        <v>312</v>
-      </c>
-      <c r="E47" s="59"/>
-      <c r="F47" s="59"/>
-      <c r="G47" s="63" t="s">
-        <v>335</v>
-      </c>
-      <c r="H47" s="63" t="s">
-        <v>328</v>
-      </c>
-      <c r="I47" s="58"/>
-      <c r="J47" s="58"/>
-      <c r="K47" s="58"/>
-      <c r="L47" s="57"/>
-      <c r="M47" s="61" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" s="60" customFormat="1" ht="270" x14ac:dyDescent="0.25">
-      <c r="A48" s="57">
-        <v>46</v>
-      </c>
-      <c r="B48" s="57" t="s">
-        <v>304</v>
-      </c>
-      <c r="C48" s="61" t="s">
-        <v>313</v>
-      </c>
-      <c r="D48" s="61" t="s">
-        <v>314</v>
-      </c>
-      <c r="E48" s="59"/>
-      <c r="F48" s="59"/>
-      <c r="G48" s="63" t="s">
-        <v>336</v>
-      </c>
-      <c r="H48" s="63" t="s">
-        <v>329</v>
-      </c>
-      <c r="I48" s="58"/>
-      <c r="J48" s="58"/>
-      <c r="K48" s="58"/>
-      <c r="L48" s="57"/>
-      <c r="M48" s="61" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" s="60" customFormat="1" ht="255" x14ac:dyDescent="0.25">
-      <c r="A49" s="57">
-        <v>47</v>
-      </c>
-      <c r="B49" s="57" t="s">
-        <v>305</v>
-      </c>
-      <c r="C49" s="61" t="s">
-        <v>315</v>
-      </c>
-      <c r="D49" s="61" t="s">
-        <v>316</v>
-      </c>
-      <c r="E49" s="59"/>
-      <c r="F49" s="59"/>
-      <c r="G49" s="63" t="s">
-        <v>337</v>
-      </c>
-      <c r="H49" s="63" t="s">
-        <v>330</v>
-      </c>
-      <c r="I49" s="58"/>
-      <c r="J49" s="58"/>
-      <c r="K49" s="58"/>
-      <c r="L49" s="57"/>
-      <c r="M49" s="61" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" s="60" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A50" s="57">
-        <v>48</v>
-      </c>
-      <c r="B50" s="57" t="s">
-        <v>306</v>
-      </c>
-      <c r="C50" s="61" t="s">
-        <v>319</v>
-      </c>
-      <c r="D50" s="61" t="s">
-        <v>326</v>
-      </c>
-      <c r="E50" s="59"/>
-      <c r="F50" s="59"/>
-      <c r="G50" s="63" t="s">
-        <v>338</v>
-      </c>
-      <c r="H50" s="63" t="s">
-        <v>331</v>
-      </c>
-      <c r="I50" s="58"/>
-      <c r="J50" s="58"/>
-      <c r="K50" s="58"/>
-      <c r="L50" s="57"/>
-      <c r="M50" s="64" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" s="60" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A51" s="57">
-        <v>49</v>
-      </c>
-      <c r="B51" s="57" t="s">
-        <v>307</v>
-      </c>
-      <c r="C51" s="61" t="s">
-        <v>320</v>
-      </c>
-      <c r="D51" s="61" t="s">
-        <v>321</v>
-      </c>
-      <c r="E51" s="59"/>
-      <c r="F51" s="59"/>
-      <c r="G51" s="63" t="s">
-        <v>339</v>
-      </c>
-      <c r="H51" s="63" t="s">
-        <v>332</v>
-      </c>
-      <c r="I51" s="58"/>
-      <c r="J51" s="58"/>
-      <c r="K51" s="58"/>
-      <c r="L51" s="57"/>
-      <c r="M51" s="61" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" s="60" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A52" s="57">
-        <v>60</v>
-      </c>
-      <c r="B52" s="57" t="s">
-        <v>308</v>
-      </c>
-      <c r="C52" s="61" t="s">
-        <v>323</v>
-      </c>
-      <c r="D52" s="61" t="s">
-        <v>322</v>
-      </c>
-      <c r="E52" s="59"/>
-      <c r="F52" s="59"/>
-      <c r="G52" s="63" t="s">
-        <v>340</v>
-      </c>
-      <c r="H52" s="63" t="s">
-        <v>333</v>
-      </c>
-      <c r="I52" s="58"/>
-      <c r="J52" s="58"/>
-      <c r="K52" s="58"/>
-      <c r="L52" s="57"/>
-      <c r="M52" s="61" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" s="60" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A53" s="57">
-        <v>51</v>
-      </c>
-      <c r="B53" s="57" t="s">
-        <v>310</v>
-      </c>
-      <c r="C53" s="61" t="s">
-        <v>349</v>
-      </c>
-      <c r="D53" s="61" t="s">
-        <v>350</v>
-      </c>
-      <c r="E53" s="59"/>
-      <c r="F53" s="59"/>
-      <c r="G53" s="63" t="s">
-        <v>387</v>
-      </c>
-      <c r="H53" s="63" t="s">
-        <v>388</v>
-      </c>
-      <c r="I53" s="58"/>
-      <c r="J53" s="58"/>
-      <c r="K53" s="58"/>
-      <c r="L53" s="57"/>
-      <c r="M53" s="64" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" s="60" customFormat="1" ht="180" x14ac:dyDescent="0.25">
-      <c r="A54" s="57">
-        <v>52</v>
-      </c>
-      <c r="B54" s="57" t="s">
-        <v>309</v>
-      </c>
-      <c r="C54" s="61" t="s">
-        <v>324</v>
-      </c>
-      <c r="D54" s="61" t="s">
-        <v>325</v>
-      </c>
-      <c r="E54" s="59"/>
-      <c r="F54" s="59"/>
-      <c r="G54" s="63" t="s">
-        <v>389</v>
-      </c>
-      <c r="H54" s="63" t="s">
-        <v>390</v>
-      </c>
-      <c r="I54" s="58"/>
-      <c r="J54" s="58"/>
-      <c r="K54" s="58"/>
-      <c r="L54" s="57"/>
-      <c r="M54" s="61" t="s">
-        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -4480,7 +4471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
@@ -4491,42 +4482,42 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>393</v>
+        <v>382</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
use different email formulation for last session: no next session
</commit_message>
<xml_diff>
--- a/actions/Activities.xlsx
+++ b/actions/Activities.xlsx
@@ -1121,9 +1121,6 @@
     <t>Changes in text from first experiment</t>
   </si>
   <si>
-    <t>As social beings, our actions are observed by those around us, who may react in various ways. To boost your confidence when preparing for becoming more physically active, it can be beneficial to envision how those who are important to you will respond to your future physically active self. This can be your colleagues, friends, family, or neighbors, for example. While their reactions may be positive, they could also be negative. So it is wise to anticipate and prepare for both possible outcomes.  Before the next session, grab a pen and paper and answer these 4 questions: 1) How would the people who are important to you react to the new you, who has become more physically active? 2) How would you feel about their reactions? 3) How would you react if the people who are important to you react positively to the new you? 4) How would you react if the people who are important to you react negatively to the new you?</t>
-  </si>
-  <si>
     <t>Number</t>
   </si>
   <si>
@@ -1706,15 +1703,6 @@
     <t>5|25</t>
   </si>
   <si>
-    <t>People are social creatures. This means that what we do is noticed by others around us, and they can react to it. To help you quit smoking, it can be useful to imagine how people who are important to you will receive your non-smoker future self. This can boost your confidence. The reactions of others, such as friends, colleagues, and family, to your future self can be positive, but they could also be negative. It is good to be prepared for both possibilities. Before the next session, grab a pen and paper and answer these 4 questions: 1) How would the people who are important to you react to the new you, who has quit smoking? 2) How would you feel about their reactions? 3) How would you react if the people who are important to you react positively to the new you? 4) How would you react if the people who are important to you react negatively to the new you?</t>
-  </si>
-  <si>
-    <t>To increase your confidence that you will succeed in quitting smoking, it can help to think back to previous successes. Have you ever quit smoking before or reduced the number of times you smoked? Maybe you once only had one instead of two cigarettes after dinner. Every success in quitting smoking counts! Before the next session, take some time to think about it and make a list on a piece of paper. Take a few minutes to make your list before moving on. Then take a closer look at your list. Try to think about what you did that helped you to achieve these things. Write it down on your list so you do not forget it. You can also hang or place your list somewhere in your home so that you are reminded of your successes more often. The list shows that you can be proud of yourself.</t>
-  </si>
-  <si>
-    <t>Reflecting on past successes can boost your confidence in successfully becoming more physically active. Before the next session, think about when you succeeded in being more physically active. Have you ever taken the bike instead of the car, or taken the stairs instead of the escalator? Every small victory counts! Take a few minutes to make your list before moving on. Then take a closer look at your list. Try to think about what you did that helped you to achieve these things. Write it down on your list so you do not forget it. You can also hang or place your list somewhere in your home so you are reminded of your successes more often. These successes show that you can be proud of yourself.</t>
-  </si>
-  <si>
     <t>Having high aspiration to quit smoking may aid in quitting successfully. Thus, before the next session, I advise you to think about the person that you would like to be once you have successfully quit smoking. For example, you might want to be a "strong woman who lives a healthy life" or a "father who is a good role model for his children." Then look for or take a picture that best captures your desired future self. Save or print this picture so that you can see it every day.</t>
   </si>
   <si>
@@ -1778,18 +1766,6 @@
     <t>Being more physically active (e.g., taking walks, swimming, or going running) may aid you to stop smoking. One important aspect for this is to have strong resolve to become more physically active. So, after this session, I advise you to take some time to create a personal rule that helps you to become more physically active. Possible examples include "10 squats - no matter what," "Say no to sitting, yes to life" or "Driving to the grocery store is NOT an option." Write down your rule on a piece of paper and repeat it to yourself 3 times. Put the piece of paper with your rule somewhere you can see it every day.</t>
   </si>
   <si>
-    <t>People are social creatures. This means that what we do is noticed by others around us, and they can react to it. To help you quit smoking, it can be useful to imagine how people who are important to you will receive your non-smoker future self. This can boost your confidence. The reactions of others, such as friends, colleagues, and family, to your future self can be positive, but they could also be negative. It is good to be prepared for both possibilities. After this session, grab a pen and paper and answer these 4 questions: 1) How would the people who are important to you react to the new you, who has quit smoking? 2) How would you feel about their reactions? 3) How would you react if the people who are important to you react positively to the new you? 4) How would you react if the people who are important to you react negatively to the new you?</t>
-  </si>
-  <si>
-    <t>As social beings, our actions are observed by those around us, who may react in various ways. To boost your confidence when preparing for becoming more physically active, it can be beneficial to envision how those who are important to you will respond to your future physically active self. This can be your colleagues, friends, family, or neighbors, for example. While their reactions may be positive, they could also be negative. So it is wise to anticipate and prepare for both possible outcomes.  After this session, grab a pen and paper and answer these 4 questions: 1) How would the people who are important to you react to the new you, who has become more physically active? 2) How would you feel about their reactions? 3) How would you react if the people who are important to you react positively to the new you? 4) How would you react if the people who are important to you react negatively to the new you?</t>
-  </si>
-  <si>
-    <t>To increase your confidence that you will succeed in quitting smoking, it can help to think back to previous successes. Have you ever quit smoking before or reduced the number of times you smoked? Maybe you once only had one instead of two cigarettes after dinner. Every success in quitting smoking counts! After this session, take some time to think about it and make a list on a piece of paper. Take a few minutes to make your list before moving on. Then take a closer look at your list. Try to think about what you did that helped you to achieve these things. Write it down on your list so you do not forget it. You can also hang or place your list somewhere in your home so that you are reminded of your successes more often. The list shows that you can be proud of yourself.</t>
-  </si>
-  <si>
-    <t>Reflecting on past successes can boost your confidence in successfully becoming more physically active. After this session, think about when you succeeded in being more physically active. Have you ever taken the bike instead of the car, or taken the stairs instead of the escalator? Every small victory counts! Take a few minutes to make your list before moving on. Then take a closer look at your list. Try to think about what you did that helped you to achieve these things. Write it down on your list so you do not forget it. You can also hang or place your list somewhere in your home so you are reminded of your successes more often. These successes show that you can be proud of yourself.</t>
-  </si>
-  <si>
     <t>Many people want to quit smoking for other people, such as children or friends. Thinking about how quitting smoking makes you a role model by doing something good for others can motivate you during difficult moments in your quitting journey. I, therefore, recommend you think about how quitting smoking makes you a role model for others after this session. Grab a pen and a piece of paper and write down your thoughts. Or maybe a picture can help you capture your thoughts.</t>
   </si>
   <si>
@@ -1880,12 +1856,6 @@
     <t>Becoming more physically active (e.g., taking walks, dancing, swimming) may help you to successfully quit smoking. One crucial part for this is to create a plan for becoming more physically active. Therefore, after this session, I advise you to think about what you could do to become more physically active. For example, you could get up from your desk after every 30 minutes of sitting, bike to the grocery store, do 10 squats every morning, or join a running group. Write down everything that comes to your mind. Which plan do you want to focus on? Highlight this plan.</t>
   </si>
   <si>
-    <t>To increase your confidence that you will succeed in changing your behavior (e.g., quitting smoking), it can help to think back to previous successes. After this session, take a moment to reflect on times when you succeeded in something or felt satisfied. Have you ever won a competition? Did you cook something delicious recently? Or maybe you learned a new language? Grab a pen and paper and make a list of your success moments. No success is too small to write down! Take a few minutes to make your list before moving on. Then take a closer look at your list. Try to think about what you did that helped you to achieve your successes. Write it down on your list so you do not forget it. You can also hang or place your list somewhere in your home so that you are reminded of your successes more often. The list shows that you can be proud of yourself.</t>
-  </si>
-  <si>
-    <t>To increase your confidence that you will succeed in changing your behavior (e.g., quitting smoking), it can help to think back to previous successes. Before the next session, take a moment to reflect on times when you succeeded in something or felt satisfied. Have you ever won a competition? Did you cook something delicious recently? Or maybe you learned a new language? Grab a pen and paper and make a list of your success moments. No success is too small to write down! Take a few minutes to make your list before moving on. Then take a closer look at your list. Try to think about what you did that helped you to achieve your successes. Write it down on your list so you do not forget it. You can also hang or place your list somewhere in your home so that you are reminded of your successes more often. The list shows that you can be proud of yourself.</t>
-  </si>
-  <si>
     <t>Adopting the right mindset is crucial in altering one's behavior (e.g., quitting smoking). It involves identifying the desired end result and having faith in one's ability to attain it. Adequate motivation and self-confidence are crucial in this process. To understand why, I recommend watching the short video that I will send you in a message on Prolific right after this session. What do you think, how can self-confidence and motivation help you to reach your end goal? Write down your thoughts on a piece of paper or your phone.</t>
   </si>
   <si>
@@ -1938,6 +1908,36 @@
   </si>
   <si>
     <t>When changing one's behavior (e.g., quitting smoking), it is possible that in the short term, one's mental and/or physical well-being decline. For example, you may sleep worse for some time after quitting smoking. Such negative effects can make it challenging to both begin and sustain your behavior change. But there are steps that you can take to minimize or even prevent such negative effects. It is useful to think about such steps when preparing to change your behavior. To understand why, I advise watching this short video before the next session: https://youtu.be/3rSqLEgRHEo. What do you think, how can learning about steps to reduce short-term negative effects on your mental and physical well-being help you to quit smoking and become more physically active? Note your thoughts on your phone or a piece of paper.</t>
+  </si>
+  <si>
+    <t>People are social creatures. This means that what we do is noticed by others around us, and they can react to it. To help you quit smoking, it can be useful to imagine how people who are important to you will receive your non-smoker future self. This can boost your confidence. The reactions of others, such as friends, colleagues, and family, to your future self can be positive, but they could also be negative. It is good to be prepared for both possibilities. After this session, I suggest you grab a pen and paper and answer these 4 questions: 1) How would the people who are important to you react to the new you, who has quit smoking? 2) How would you feel about their reactions? 3) How would you react if the people who are important to you react positively to the new you? 4) How would you react if the people who are important to you react negatively to the new you?</t>
+  </si>
+  <si>
+    <t>People are social creatures. This means that what we do is noticed by others around us, and they can react to it. To help you quit smoking, it can be useful to imagine how people who are important to you will receive your non-smoker future self. This can boost your confidence. The reactions of others, such as friends, colleagues, and family, to your future self can be positive, but they could also be negative. It is good to be prepared for both possibilities. Before the next session, I suggest you grab a pen and paper and answer these 4 questions: 1) How would the people who are important to you react to the new you, who has quit smoking? 2) How would you feel about their reactions? 3) How would you react if the people who are important to you react positively to the new you? 4) How would you react if the people who are important to you react negatively to the new you?</t>
+  </si>
+  <si>
+    <t>As social beings, our actions are observed by those around us, who may react in various ways. To boost your confidence when preparing for becoming more physically active, it can be beneficial to envision how those who are important to you will respond to your future physically active self. This can be your colleagues, friends, family, or neighbors, for example. While their reactions may be positive, they could also be negative. So it is wise to anticipate and prepare for both possible outcomes.  After this session, I suggest you grab a pen and paper and answer these 4 questions: 1) How would the people who are important to you react to the new you, who has become more physically active? 2) How would you feel about their reactions? 3) How would you react if the people who are important to you react positively to the new you? 4) How would you react if the people who are important to you react negatively to the new you?</t>
+  </si>
+  <si>
+    <t>As social beings, our actions are observed by those around us, who may react in various ways. To boost your confidence when preparing for becoming more physically active, it can be beneficial to envision how those who are important to you will respond to your future physically active self. This can be your colleagues, friends, family, or neighbors, for example. While their reactions may be positive, they could also be negative. So it is wise to anticipate and prepare for both possible outcomes.  Before the next session, I suggest you grab a pen and paper and answer these 4 questions: 1) How would the people who are important to you react to the new you, who has become more physically active? 2) How would you feel about their reactions? 3) How would you react if the people who are important to you react positively to the new you? 4) How would you react if the people who are important to you react negatively to the new you?</t>
+  </si>
+  <si>
+    <t>To increase your confidence that you will succeed in quitting smoking, it can help to think back to previous successes. Have you ever quit smoking before or reduced the number of times you smoked? Maybe you once only had one instead of two cigarettes after dinner. Every success in quitting smoking counts! After this session, I suggest you take some time to think about you previous successes and make a list on a piece of paper. Take a few minutes to make your list before moving on. Then take a closer look at your list. Try to think about what strengths you have that helped you to achieve these things. Write these strengths down on your list so you do not forget them. You can also hang or place your list somewhere in your home so that you are reminded of your successes and strengths more often. The list shows that you can be proud of yourself.</t>
+  </si>
+  <si>
+    <t>To increase your confidence that you will succeed in quitting smoking, it can help to think back to previous successes. Have you ever quit smoking before or reduced the number of times you smoked? Maybe you once only had one instead of two cigarettes after dinner. Every success in quitting smoking counts! Before the next session, I suggest you take some time to think about your previous successes and make a list on a piece of paper. Take a few minutes to make your list before moving on. Then take a closer look at your list. Try to think about what strengths you have that helped you to achieve these things. Write these strengths down on your list so you do not forget them. You can also hang or place your list somewhere in your home so that you are reminded of your successes and strengths more often. The list shows that you can be proud of yourself.</t>
+  </si>
+  <si>
+    <t>Reflecting on past successes can boost your confidence in successfully becoming more physically active. After this session, I suggest you think about when you succeeded in being more physically active. Have you ever taken the bike instead of the car, or taken the stairs instead of the escalator? Every small victory counts! Take a few minutes to make your list before moving on. Then take a closer look at your list. Try to think about what you did that helped you to achieve these things. Write it down on your list so you do not forget it. You can also hang or place your list somewhere in your home so you are reminded of your successes more often. These successes show that you can be proud of yourself.</t>
+  </si>
+  <si>
+    <t>Reflecting on past successes can boost your confidence in successfully becoming more physically active. Before the next session, I suggest you think about when you succeeded in being more physically active. Have you ever taken the bike instead of the car, or taken the stairs instead of the escalator? Every small victory counts! Take a few minutes to make your list before moving on. Then take a closer look at your list. Try to think about what you did that helped you to achieve these things. Write it down on your list so you do not forget it. You can also hang or place your list somewhere in your home so you are reminded of your successes more often. These successes show that you can be proud of yourself.</t>
+  </si>
+  <si>
+    <t>To increase your confidence that you will succeed in changing your behavior (e.g., quitting smoking), it can help to think back to previous successes. After this session, I suggest you take a moment to reflect on times when you succeeded in something or felt satisfied. Have you ever won a competition? Did you cook something delicious recently? Or maybe you learned a new language? Grab a pen and paper and make a list of your success moments. No success is too small to write down! Take a few minutes to make your list before moving on. Then take a closer look at your list. Try to think about what you did that helped you to achieve your successes. Write it down on your list so you do not forget it. You can also hang or place your list somewhere in your home so that you are reminded of your successes more often. The list shows that you can be proud of yourself.</t>
+  </si>
+  <si>
+    <t>To increase your confidence that you will succeed in changing your behavior (e.g., quitting smoking), it can help to think back to previous successes. Before the next session, I suggest you take a moment to reflect on times when you succeeded in something or felt satisfied. Have you ever won a competition? Did you cook something delicious recently? Or maybe you learned a new language? Grab a pen and paper and make a list of your success moments. No success is too small to write down! Take a few minutes to make your list before moving on. Then take a closer look at your list. Try to think about what you did that helped you to achieve your successes. Write it down on your list so you do not forget it. You can also hang or place your list somewhere in your home so that you are reminded of your successes more often. The list shows that you can be proud of yourself.</t>
   </si>
 </sst>
 </file>
@@ -2585,7 +2585,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>128</v>
@@ -2594,19 +2594,19 @@
         <v>129</v>
       </c>
       <c r="D1" s="61" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E1" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>210</v>
-      </c>
       <c r="G1" s="54" t="s">
+        <v>300</v>
+      </c>
+      <c r="H1" s="52" t="s">
         <v>301</v>
-      </c>
-      <c r="H1" s="52" t="s">
-        <v>302</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>206</v>
@@ -2635,14 +2635,14 @@
         <v>107</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10">
         <v>1</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="H2" s="11" t="s">
         <v>177</v>
@@ -2668,14 +2668,14 @@
         <v>126</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="15">
         <v>0</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="H3" s="11" t="s">
         <v>178</v>
@@ -2701,17 +2701,17 @@
         <v>89</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E4" s="10"/>
       <c r="F4" s="10">
         <v>3</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="I4" s="9"/>
       <c r="J4" s="18" t="s">
@@ -2736,17 +2736,17 @@
         <v>112</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="15">
         <v>2</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="I5" s="14"/>
       <c r="J5" s="16"/>
@@ -2769,14 +2769,14 @@
         <v>123</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="10" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G6" s="21" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="H6" s="21" t="s">
         <v>133</v>
@@ -2806,14 +2806,14 @@
         <v>124</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G7" s="21" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="H7" s="21" t="s">
         <v>135</v>
@@ -2843,12 +2843,12 @@
         <v>37</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
       <c r="G8" s="11" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="H8" s="11" t="s">
         <v>137</v>
@@ -2880,12 +2880,12 @@
         <v>50</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
       <c r="G9" s="21" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="H9" s="21" t="s">
         <v>139</v>
@@ -2915,14 +2915,14 @@
         <v>75</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="10">
         <v>9</v>
       </c>
       <c r="G10" s="21" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="H10" s="21" t="s">
         <v>9</v>
@@ -2952,14 +2952,14 @@
         <v>81</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="15">
         <v>8</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="H11" s="11" t="s">
         <v>142</v>
@@ -2989,19 +2989,19 @@
         <v>104</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F12" s="10">
         <v>11</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>340</v>
+        <v>384</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>316</v>
+        <v>385</v>
       </c>
       <c r="I12" s="9"/>
       <c r="J12" s="12"/>
@@ -3015,7 +3015,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="225" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="240" x14ac:dyDescent="0.25">
       <c r="A13" s="51">
         <v>11</v>
       </c>
@@ -3026,19 +3026,19 @@
         <v>105</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F13" s="15">
         <v>10</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>341</v>
+        <v>386</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>207</v>
+        <v>387</v>
       </c>
       <c r="I13" s="14"/>
       <c r="J13" s="16"/>
@@ -3050,7 +3050,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="195" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="210" x14ac:dyDescent="0.25">
       <c r="A14" s="51">
         <v>12</v>
       </c>
@@ -3061,17 +3061,17 @@
         <v>127</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="10" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>342</v>
+        <v>388</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>317</v>
+        <v>389</v>
       </c>
       <c r="I14" s="9"/>
       <c r="J14" s="12"/>
@@ -3096,17 +3096,17 @@
         <v>60</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E15" s="15"/>
       <c r="F15" s="15" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>343</v>
+        <v>390</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>318</v>
+        <v>391</v>
       </c>
       <c r="I15" s="14"/>
       <c r="J15" s="16"/>
@@ -3128,20 +3128,20 @@
         <v>108</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="10">
         <v>15</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="I16" s="9"/>
       <c r="J16" s="12"/>
@@ -3163,20 +3163,20 @@
         <v>114</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E17" s="15"/>
       <c r="F17" s="15">
         <v>14</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="I17" s="14"/>
       <c r="J17" s="16"/>
@@ -3199,12 +3199,12 @@
         <v>77</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="11" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="H18" s="11" t="s">
         <v>11</v>
@@ -3234,12 +3234,12 @@
         <v>78</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
       <c r="G19" s="11" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="H19" s="11" t="s">
         <v>143</v>
@@ -3269,14 +3269,14 @@
         <v>118</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="10" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="H20" s="11" t="s">
         <v>145</v>
@@ -3306,14 +3306,14 @@
         <v>117</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E21" s="15"/>
       <c r="F21" s="15" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="H21" s="11" t="s">
         <v>147</v>
@@ -3343,14 +3343,14 @@
         <v>120</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="10" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="H22" s="11" t="s">
         <v>148</v>
@@ -3380,14 +3380,14 @@
         <v>119</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E23" s="15"/>
       <c r="F23" s="15" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="H23" s="11" t="s">
         <v>150</v>
@@ -3417,14 +3417,14 @@
         <v>109</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E24" s="10"/>
       <c r="F24" s="10">
         <v>23</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="H24" s="11" t="s">
         <v>151</v>
@@ -3454,14 +3454,14 @@
         <v>92</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E25" s="15"/>
       <c r="F25" s="15">
         <v>22</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="H25" s="11" t="s">
         <v>153</v>
@@ -3491,17 +3491,17 @@
         <v>121</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E26" s="10"/>
       <c r="F26" s="10" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G26" s="21" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="H26" s="21" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="I26" s="9" t="s">
         <v>166</v>
@@ -3526,14 +3526,14 @@
         <v>122</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E27" s="15"/>
       <c r="F27" s="15" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="H27" s="11" t="s">
         <v>154</v>
@@ -3563,15 +3563,15 @@
         <v>86</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E28" s="31"/>
       <c r="F28" s="31"/>
       <c r="G28" s="11" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="H28" s="11" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="I28" s="30"/>
       <c r="J28" s="30" t="s">
@@ -3598,15 +3598,15 @@
         <v>88</v>
       </c>
       <c r="D29" s="30" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E29" s="31"/>
       <c r="F29" s="31"/>
       <c r="G29" s="11" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="H29" s="11" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="I29" s="30"/>
       <c r="J29" s="30" t="s">
@@ -3631,14 +3631,14 @@
         <v>42</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E30" s="31">
         <v>16</v>
       </c>
       <c r="F30" s="31"/>
       <c r="G30" s="21" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="H30" s="21" t="s">
         <v>5</v>
@@ -3668,14 +3668,14 @@
         <v>72</v>
       </c>
       <c r="D31" s="30" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E31" s="31">
         <v>16</v>
       </c>
       <c r="F31" s="31"/>
       <c r="G31" s="11" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="H31" s="11" t="s">
         <v>156</v>
@@ -3705,12 +3705,12 @@
         <v>73</v>
       </c>
       <c r="D32" s="30" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E32" s="31"/>
       <c r="F32" s="31"/>
       <c r="G32" s="21" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="H32" s="21" t="s">
         <v>7</v>
@@ -3742,14 +3742,14 @@
         <v>74</v>
       </c>
       <c r="D33" s="30" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E33" s="31"/>
       <c r="F33" s="31">
         <v>32</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="H33" s="11" t="s">
         <v>157</v>
@@ -3779,17 +3779,17 @@
         <v>83</v>
       </c>
       <c r="D34" s="30" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E34" s="31"/>
       <c r="F34" s="31">
         <v>31</v>
       </c>
       <c r="G34" s="11" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="H34" s="11" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="I34" s="30"/>
       <c r="J34" s="37" t="s">
@@ -3814,17 +3814,17 @@
         <v>84</v>
       </c>
       <c r="D35" s="30" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E35" s="31">
         <v>34</v>
       </c>
       <c r="F35" s="31"/>
       <c r="G35" s="11" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="H35" s="11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I35" s="30"/>
       <c r="J35" s="30" t="s">
@@ -3849,15 +3849,15 @@
         <v>85</v>
       </c>
       <c r="D36" s="30" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E36" s="31"/>
       <c r="F36" s="31"/>
       <c r="G36" s="11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H36" s="11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I36" s="30"/>
       <c r="J36" s="30" t="s">
@@ -3882,15 +3882,15 @@
         <v>87</v>
       </c>
       <c r="D37" s="30" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E37" s="31"/>
       <c r="F37" s="31"/>
       <c r="G37" s="11" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="H37" s="11" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="I37" s="30"/>
       <c r="J37" s="37" t="s">
@@ -3915,12 +3915,12 @@
         <v>76</v>
       </c>
       <c r="D38" s="30" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E38" s="31"/>
       <c r="F38" s="31"/>
       <c r="G38" s="11" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="H38" s="11" t="s">
         <v>159</v>
@@ -3950,12 +3950,12 @@
         <v>82</v>
       </c>
       <c r="D39" s="40" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E39" s="41"/>
       <c r="F39" s="41"/>
       <c r="G39" s="11" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="H39" s="11" t="s">
         <v>173</v>
@@ -3983,15 +3983,15 @@
         <v>57</v>
       </c>
       <c r="D40" s="40" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E40" s="41"/>
       <c r="F40" s="41"/>
       <c r="G40" s="11" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="H40" s="11" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="I40" s="40" t="s">
         <v>198</v>
@@ -4020,12 +4020,12 @@
         <v>79</v>
       </c>
       <c r="D41" s="40" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E41" s="41"/>
       <c r="F41" s="41"/>
       <c r="G41" s="11" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="H41" s="11" t="s">
         <v>160</v>
@@ -4057,14 +4057,14 @@
         <v>51</v>
       </c>
       <c r="D42" s="40" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E42" s="41">
         <v>17</v>
       </c>
       <c r="F42" s="41"/>
       <c r="G42" s="11" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="H42" s="11" t="s">
         <v>161</v>
@@ -4094,14 +4094,14 @@
         <v>80</v>
       </c>
       <c r="D43" s="40" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E43" s="41">
         <v>17</v>
       </c>
       <c r="F43" s="41"/>
       <c r="G43" s="11" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="H43" s="11" t="s">
         <v>162</v>
@@ -4131,15 +4131,15 @@
         <v>125</v>
       </c>
       <c r="D44" s="45" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E44" s="46"/>
       <c r="F44" s="46"/>
       <c r="G44" s="11" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="H44" s="11" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="I44" s="45"/>
       <c r="J44" s="47"/>
@@ -4162,17 +4162,17 @@
         <v>116</v>
       </c>
       <c r="D45" s="45" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E45" s="46"/>
       <c r="F45" s="46" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G45" s="11" t="s">
-        <v>374</v>
+        <v>392</v>
       </c>
       <c r="H45" s="11" t="s">
-        <v>375</v>
+        <v>393</v>
       </c>
       <c r="I45" s="45"/>
       <c r="J45" s="47"/>
@@ -4191,28 +4191,28 @@
         <v>44</v>
       </c>
       <c r="B46" s="56" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C46" s="60" t="s">
+        <v>280</v>
+      </c>
+      <c r="D46" s="60" t="s">
         <v>281</v>
-      </c>
-      <c r="D46" s="60" t="s">
-        <v>282</v>
       </c>
       <c r="E46" s="58"/>
       <c r="F46" s="58"/>
       <c r="G46" s="62" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
       <c r="H46" s="62" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="I46" s="57"/>
       <c r="J46" s="57"/>
       <c r="K46" s="57"/>
       <c r="L46" s="56"/>
       <c r="M46" s="60" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="47" spans="1:13" s="59" customFormat="1" ht="225" x14ac:dyDescent="0.25">
@@ -4220,28 +4220,28 @@
         <v>45</v>
       </c>
       <c r="B47" s="56" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C47" s="60" t="s">
+        <v>274</v>
+      </c>
+      <c r="D47" s="60" t="s">
         <v>275</v>
-      </c>
-      <c r="D47" s="60" t="s">
-        <v>276</v>
       </c>
       <c r="E47" s="58"/>
       <c r="F47" s="58"/>
       <c r="G47" s="62" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="H47" s="62" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="I47" s="57"/>
       <c r="J47" s="57"/>
       <c r="K47" s="57"/>
       <c r="L47" s="56"/>
       <c r="M47" s="60" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="48" spans="1:13" s="59" customFormat="1" ht="270" x14ac:dyDescent="0.25">
@@ -4249,28 +4249,28 @@
         <v>46</v>
       </c>
       <c r="B48" s="56" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C48" s="60" t="s">
+        <v>276</v>
+      </c>
+      <c r="D48" s="60" t="s">
         <v>277</v>
-      </c>
-      <c r="D48" s="60" t="s">
-        <v>278</v>
       </c>
       <c r="E48" s="58"/>
       <c r="F48" s="58"/>
       <c r="G48" s="62" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="H48" s="62" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="I48" s="57"/>
       <c r="J48" s="57"/>
       <c r="K48" s="57"/>
       <c r="L48" s="56"/>
       <c r="M48" s="60" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="49" spans="1:13" s="59" customFormat="1" ht="255" x14ac:dyDescent="0.25">
@@ -4278,28 +4278,28 @@
         <v>47</v>
       </c>
       <c r="B49" s="56" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C49" s="60" t="s">
+        <v>278</v>
+      </c>
+      <c r="D49" s="60" t="s">
         <v>279</v>
-      </c>
-      <c r="D49" s="60" t="s">
-        <v>280</v>
       </c>
       <c r="E49" s="58"/>
       <c r="F49" s="58"/>
       <c r="G49" s="62" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="H49" s="62" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
       <c r="I49" s="57"/>
       <c r="J49" s="57"/>
       <c r="K49" s="57"/>
       <c r="L49" s="56"/>
       <c r="M49" s="60" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="50" spans="1:13" s="59" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -4307,28 +4307,28 @@
         <v>48</v>
       </c>
       <c r="B50" s="56" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C50" s="60" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D50" s="60" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E50" s="58"/>
       <c r="F50" s="58"/>
       <c r="G50" s="62" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
       <c r="H50" s="62" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="I50" s="57"/>
       <c r="J50" s="57"/>
       <c r="K50" s="57"/>
       <c r="L50" s="56"/>
       <c r="M50" s="63" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="51" spans="1:13" s="59" customFormat="1" ht="120" x14ac:dyDescent="0.25">
@@ -4336,21 +4336,21 @@
         <v>49</v>
       </c>
       <c r="B51" s="56" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C51" s="60" t="s">
+        <v>283</v>
+      </c>
+      <c r="D51" s="60" t="s">
         <v>284</v>
-      </c>
-      <c r="D51" s="60" t="s">
-        <v>285</v>
       </c>
       <c r="E51" s="58"/>
       <c r="F51" s="58"/>
       <c r="G51" s="62" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="H51" s="62" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
       <c r="I51" s="57"/>
       <c r="J51" s="57"/>
@@ -4365,28 +4365,28 @@
         <v>60</v>
       </c>
       <c r="B52" s="56" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C52" s="60" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D52" s="60" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E52" s="58"/>
       <c r="F52" s="58"/>
       <c r="G52" s="62" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="H52" s="62" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="I52" s="57"/>
       <c r="J52" s="57"/>
       <c r="K52" s="57"/>
       <c r="L52" s="56"/>
       <c r="M52" s="60" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="53" spans="1:13" s="59" customFormat="1" ht="165" x14ac:dyDescent="0.25">
@@ -4394,28 +4394,28 @@
         <v>51</v>
       </c>
       <c r="B53" s="56" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C53" s="60" t="s">
+        <v>298</v>
+      </c>
+      <c r="D53" s="60" t="s">
         <v>299</v>
-      </c>
-      <c r="D53" s="60" t="s">
-        <v>300</v>
       </c>
       <c r="E53" s="58"/>
       <c r="F53" s="58"/>
       <c r="G53" s="62" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="H53" s="62" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="I53" s="57"/>
       <c r="J53" s="57"/>
       <c r="K53" s="57"/>
       <c r="L53" s="56"/>
       <c r="M53" s="63" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="54" spans="1:13" s="59" customFormat="1" ht="210" x14ac:dyDescent="0.25">
@@ -4423,28 +4423,28 @@
         <v>52</v>
       </c>
       <c r="B54" s="56" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C54" s="60" t="s">
+        <v>287</v>
+      </c>
+      <c r="D54" s="60" t="s">
         <v>288</v>
-      </c>
-      <c r="D54" s="60" t="s">
-        <v>289</v>
       </c>
       <c r="E54" s="58"/>
       <c r="F54" s="58"/>
       <c r="G54" s="62" t="s">
-        <v>392</v>
+        <v>382</v>
       </c>
       <c r="H54" s="62" t="s">
-        <v>393</v>
+        <v>383</v>
       </c>
       <c r="I54" s="57"/>
       <c r="J54" s="57"/>
       <c r="K54" s="57"/>
       <c r="L54" s="56"/>
       <c r="M54" s="60" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -4482,42 +4482,42 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adapted activity verbs + state questions
</commit_message>
<xml_diff>
--- a/actions/Activities.xlsx
+++ b/actions/Activities.xlsx
@@ -1310,18 +1310,6 @@
     <t>U5 Motivation to change</t>
   </si>
   <si>
-    <t>U6 Knowledge mental well-being</t>
-  </si>
-  <si>
-    <t>U7 Physical activity helps to quit smoking</t>
-  </si>
-  <si>
-    <t>U9 Knowledge well-being</t>
-  </si>
-  <si>
-    <t>U8 Awareness of obstacles</t>
-  </si>
-  <si>
     <t>Learning about the usefulness of practical preparation to successfully change one's behavior</t>
   </si>
   <si>
@@ -1652,12 +1640,6 @@
     </r>
   </si>
   <si>
-    <t>Learning about the usefulness of being aware of possible obstacles to succeed in changing one's behavior</t>
-  </si>
-  <si>
-    <t>learn about the usefulness of being aware of possible obstacles to succeed in changing your behavior</t>
-  </si>
-  <si>
     <t>Formulation Session</t>
   </si>
   <si>
@@ -1938,6 +1920,24 @@
   </si>
   <si>
     <t>To increase your confidence that you will succeed in changing your behavior (e.g., quitting smoking), it can help to think back to previous successes. Before the next session, I suggest you take a moment to reflect on times when you succeeded in something or felt satisfied. Have you ever won a competition? Did you cook something delicious recently? Or maybe you learned a new language? Grab a pen and paper and make a list of your success moments. No success is too small to write down! Take a few minutes to make your list before moving on. Then take a closer look at your list. Try to think about what you did that helped you to achieve your successes. Write it down on your list so you do not forget it. You can also hang or place your list somewhere in your home so that you are reminded of your successes more often. The list shows that you can be proud of yourself.</t>
+  </si>
+  <si>
+    <t>U6 Knowledge how to maintain/achieve mental well-being</t>
+  </si>
+  <si>
+    <t>U7 Mindset that physical activity helps to quit smoking</t>
+  </si>
+  <si>
+    <t>U8 Awareness of smoking patterns</t>
+  </si>
+  <si>
+    <t>Learning about how thinking of possible obstacles is useful to succeed in changing one's behavior</t>
+  </si>
+  <si>
+    <t>learn about how thinking of possible obstaclesis useful  to succeed in changing your behavior</t>
+  </si>
+  <si>
+    <t>U9 Knowledge how to maintain/achieve well-being</t>
   </si>
 </sst>
 </file>
@@ -1990,7 +1990,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2012,18 +2012,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2074,21 +2062,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -2098,7 +2086,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2124,7 +2112,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2151,49 +2139,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -2213,37 +2158,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2565,21 +2522,21 @@
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomLeft" activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="51"/>
+    <col min="1" max="1" width="9.140625" style="36"/>
     <col min="2" max="2" width="40.42578125" style="8" customWidth="1"/>
     <col min="3" max="4" width="60.28515625" style="24" customWidth="1"/>
-    <col min="5" max="6" width="60.28515625" style="50" customWidth="1"/>
-    <col min="7" max="7" width="60.28515625" style="55" customWidth="1"/>
-    <col min="8" max="8" width="60.28515625" style="53" customWidth="1"/>
+    <col min="5" max="6" width="60.28515625" style="35" customWidth="1"/>
+    <col min="7" max="7" width="60.28515625" style="40" customWidth="1"/>
+    <col min="8" max="8" width="60.28515625" style="38" customWidth="1"/>
     <col min="9" max="9" width="60.28515625" style="8" customWidth="1"/>
     <col min="10" max="10" width="50.140625" style="8" customWidth="1"/>
     <col min="11" max="11" width="59.85546875" style="8" customWidth="1"/>
-    <col min="12" max="12" width="57.28515625" style="51" customWidth="1"/>
+    <col min="12" max="12" width="57.28515625" style="36" customWidth="1"/>
     <col min="13" max="13" width="55.28515625" style="24" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2590,10 +2547,10 @@
       <c r="B1" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="C1" s="61" t="s">
+      <c r="C1" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="D1" s="61" t="s">
+      <c r="D1" s="46" t="s">
         <v>219</v>
       </c>
       <c r="E1" s="6" t="s">
@@ -2602,11 +2559,11 @@
       <c r="F1" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="G1" s="54" t="s">
-        <v>300</v>
-      </c>
-      <c r="H1" s="52" t="s">
-        <v>301</v>
+      <c r="G1" s="39" t="s">
+        <v>294</v>
+      </c>
+      <c r="H1" s="37" t="s">
+        <v>295</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>206</v>
@@ -2620,12 +2577,12 @@
       <c r="L1" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="M1" s="61" t="s">
+      <c r="M1" s="46" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="105" x14ac:dyDescent="0.25">
-      <c r="A2" s="51">
+      <c r="A2" s="36">
         <v>0</v>
       </c>
       <c r="B2" s="9" t="s">
@@ -2642,7 +2599,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="H2" s="11" t="s">
         <v>177</v>
@@ -2658,7 +2615,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="105" x14ac:dyDescent="0.25">
-      <c r="A3" s="51">
+      <c r="A3" s="36">
         <v>1</v>
       </c>
       <c r="B3" s="14" t="s">
@@ -2675,7 +2632,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="H3" s="11" t="s">
         <v>178</v>
@@ -2691,7 +2648,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="210" x14ac:dyDescent="0.25">
-      <c r="A4" s="51">
+      <c r="A4" s="36">
         <v>2</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -2708,10 +2665,10 @@
         <v>3</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="I4" s="9"/>
       <c r="J4" s="18" t="s">
@@ -2726,7 +2683,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="150" x14ac:dyDescent="0.25">
-      <c r="A5" s="51">
+      <c r="A5" s="36">
         <v>3</v>
       </c>
       <c r="B5" s="14" t="s">
@@ -2743,10 +2700,10 @@
         <v>2</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="I5" s="14"/>
       <c r="J5" s="16"/>
@@ -2759,7 +2716,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="210" x14ac:dyDescent="0.25">
-      <c r="A6" s="51">
+      <c r="A6" s="36">
         <v>4</v>
       </c>
       <c r="B6" s="9" t="s">
@@ -2773,10 +2730,10 @@
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="10" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="G6" s="21" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="H6" s="21" t="s">
         <v>133</v>
@@ -2796,7 +2753,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="210" x14ac:dyDescent="0.25">
-      <c r="A7" s="51">
+      <c r="A7" s="36">
         <v>5</v>
       </c>
       <c r="B7" s="14" t="s">
@@ -2810,10 +2767,10 @@
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="15" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="G7" s="21" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="H7" s="21" t="s">
         <v>135</v>
@@ -2833,7 +2790,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="195" x14ac:dyDescent="0.25">
-      <c r="A8" s="51">
+      <c r="A8" s="36">
         <v>6</v>
       </c>
       <c r="B8" s="9" t="s">
@@ -2848,7 +2805,7 @@
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
       <c r="G8" s="11" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="H8" s="11" t="s">
         <v>137</v>
@@ -2870,7 +2827,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="150" x14ac:dyDescent="0.25">
-      <c r="A9" s="51">
+      <c r="A9" s="36">
         <v>7</v>
       </c>
       <c r="B9" s="14" t="s">
@@ -2885,7 +2842,7 @@
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
       <c r="G9" s="21" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="H9" s="21" t="s">
         <v>139</v>
@@ -2905,7 +2862,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="150" x14ac:dyDescent="0.25">
-      <c r="A10" s="51">
+      <c r="A10" s="36">
         <v>8</v>
       </c>
       <c r="B10" s="9" t="s">
@@ -2922,7 +2879,7 @@
         <v>9</v>
       </c>
       <c r="G10" s="21" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="H10" s="21" t="s">
         <v>9</v>
@@ -2942,7 +2899,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="195" x14ac:dyDescent="0.25">
-      <c r="A11" s="51">
+      <c r="A11" s="36">
         <v>9</v>
       </c>
       <c r="B11" s="14" t="s">
@@ -2959,7 +2916,7 @@
         <v>8</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="H11" s="11" t="s">
         <v>142</v>
@@ -2979,7 +2936,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="225" x14ac:dyDescent="0.25">
-      <c r="A12" s="51">
+      <c r="A12" s="36">
         <v>10</v>
       </c>
       <c r="B12" s="9" t="s">
@@ -2992,16 +2949,16 @@
         <v>230</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="F12" s="10">
         <v>11</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="I12" s="9"/>
       <c r="J12" s="12"/>
@@ -3016,7 +2973,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" ht="240" x14ac:dyDescent="0.25">
-      <c r="A13" s="51">
+      <c r="A13" s="36">
         <v>11</v>
       </c>
       <c r="B13" s="14" t="s">
@@ -3029,16 +2986,16 @@
         <v>231</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="F13" s="15">
         <v>10</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="I13" s="14"/>
       <c r="J13" s="16"/>
@@ -3051,7 +3008,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="210" x14ac:dyDescent="0.25">
-      <c r="A14" s="51">
+      <c r="A14" s="36">
         <v>12</v>
       </c>
       <c r="B14" s="9" t="s">
@@ -3065,13 +3022,13 @@
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="10" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="I14" s="9"/>
       <c r="J14" s="12"/>
@@ -3086,7 +3043,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="180" x14ac:dyDescent="0.25">
-      <c r="A15" s="51">
+      <c r="A15" s="36">
         <v>13</v>
       </c>
       <c r="B15" s="14" t="s">
@@ -3100,13 +3057,13 @@
       </c>
       <c r="E15" s="15"/>
       <c r="F15" s="15" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="I15" s="14"/>
       <c r="J15" s="16"/>
@@ -3121,14 +3078,14 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="225" x14ac:dyDescent="0.25">
-      <c r="A16" s="51">
+      <c r="A16" s="36">
         <v>14</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>108</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>233</v>
@@ -3138,10 +3095,10 @@
         <v>15</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="I16" s="9"/>
       <c r="J16" s="12"/>
@@ -3156,14 +3113,14 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="135" x14ac:dyDescent="0.25">
-      <c r="A17" s="51">
+      <c r="A17" s="36">
         <v>15</v>
       </c>
       <c r="B17" s="14" t="s">
         <v>114</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>234</v>
@@ -3173,10 +3130,10 @@
         <v>14</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="I17" s="14"/>
       <c r="J17" s="16"/>
@@ -3189,7 +3146,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="150" x14ac:dyDescent="0.25">
-      <c r="A18" s="51">
+      <c r="A18" s="36">
         <v>16</v>
       </c>
       <c r="B18" s="9" t="s">
@@ -3204,7 +3161,7 @@
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="11" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="H18" s="11" t="s">
         <v>11</v>
@@ -3224,7 +3181,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="210" x14ac:dyDescent="0.25">
-      <c r="A19" s="51">
+      <c r="A19" s="36">
         <v>17</v>
       </c>
       <c r="B19" s="14" t="s">
@@ -3239,7 +3196,7 @@
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
       <c r="G19" s="11" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="H19" s="11" t="s">
         <v>143</v>
@@ -3259,7 +3216,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" ht="150" x14ac:dyDescent="0.25">
-      <c r="A20" s="51">
+      <c r="A20" s="36">
         <v>18</v>
       </c>
       <c r="B20" s="9" t="s">
@@ -3273,10 +3230,10 @@
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="10" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="H20" s="11" t="s">
         <v>145</v>
@@ -3296,7 +3253,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="210" x14ac:dyDescent="0.25">
-      <c r="A21" s="51">
+      <c r="A21" s="36">
         <v>19</v>
       </c>
       <c r="B21" s="14" t="s">
@@ -3310,10 +3267,10 @@
       </c>
       <c r="E21" s="15"/>
       <c r="F21" s="15" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="H21" s="11" t="s">
         <v>147</v>
@@ -3333,7 +3290,7 @@
       </c>
     </row>
     <row r="22" spans="1:13" ht="210" x14ac:dyDescent="0.25">
-      <c r="A22" s="51">
+      <c r="A22" s="36">
         <v>20</v>
       </c>
       <c r="B22" s="9" t="s">
@@ -3347,10 +3304,10 @@
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="10" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="H22" s="11" t="s">
         <v>148</v>
@@ -3370,7 +3327,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" ht="225" x14ac:dyDescent="0.25">
-      <c r="A23" s="51">
+      <c r="A23" s="36">
         <v>21</v>
       </c>
       <c r="B23" s="14" t="s">
@@ -3384,10 +3341,10 @@
       </c>
       <c r="E23" s="15"/>
       <c r="F23" s="15" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="H23" s="11" t="s">
         <v>150</v>
@@ -3407,7 +3364,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" ht="150" x14ac:dyDescent="0.25">
-      <c r="A24" s="51">
+      <c r="A24" s="36">
         <v>22</v>
       </c>
       <c r="B24" s="9" t="s">
@@ -3424,7 +3381,7 @@
         <v>23</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="H24" s="11" t="s">
         <v>151</v>
@@ -3444,7 +3401,7 @@
       </c>
     </row>
     <row r="25" spans="1:13" ht="180" x14ac:dyDescent="0.25">
-      <c r="A25" s="51">
+      <c r="A25" s="36">
         <v>23</v>
       </c>
       <c r="B25" s="14" t="s">
@@ -3461,7 +3418,7 @@
         <v>22</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="H25" s="11" t="s">
         <v>153</v>
@@ -3481,7 +3438,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" ht="210" x14ac:dyDescent="0.25">
-      <c r="A26" s="51">
+      <c r="A26" s="36">
         <v>24</v>
       </c>
       <c r="B26" s="9" t="s">
@@ -3495,13 +3452,13 @@
       </c>
       <c r="E26" s="10"/>
       <c r="F26" s="10" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="G26" s="21" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="H26" s="21" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="I26" s="9" t="s">
         <v>166</v>
@@ -3516,7 +3473,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" ht="210" x14ac:dyDescent="0.25">
-      <c r="A27" s="51">
+      <c r="A27" s="36">
         <v>25</v>
       </c>
       <c r="B27" s="14" t="s">
@@ -3530,10 +3487,10 @@
       </c>
       <c r="E27" s="15"/>
       <c r="F27" s="15" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="H27" s="11" t="s">
         <v>154</v>
@@ -3553,898 +3510,898 @@
       </c>
     </row>
     <row r="28" spans="1:13" ht="225" x14ac:dyDescent="0.25">
-      <c r="A28" s="51">
+      <c r="A28" s="36">
         <v>26</v>
       </c>
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="30" t="s">
+      <c r="C28" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="D28" s="30" t="s">
+      <c r="D28" s="9" t="s">
         <v>245</v>
       </c>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
       <c r="G28" s="11" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="H28" s="11" t="s">
-        <v>351</v>
-      </c>
-      <c r="I28" s="30"/>
-      <c r="J28" s="30" t="s">
+        <v>345</v>
+      </c>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="K28" s="32" t="s">
+      <c r="K28" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="L28" s="33" t="s">
+      <c r="L28" s="49" t="s">
         <v>167</v>
       </c>
-      <c r="M28" s="24" t="s">
+      <c r="M28" s="9" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="135" x14ac:dyDescent="0.25">
-      <c r="A29" s="51">
+      <c r="A29" s="36">
         <v>27</v>
       </c>
-      <c r="B29" s="30" t="s">
+      <c r="B29" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="30" t="s">
+      <c r="C29" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D29" s="30" t="s">
+      <c r="D29" s="9" t="s">
         <v>246</v>
       </c>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
       <c r="G29" s="11" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="H29" s="11" t="s">
-        <v>316</v>
-      </c>
-      <c r="I29" s="30"/>
-      <c r="J29" s="30" t="s">
+        <v>310</v>
+      </c>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="K29" s="34"/>
-      <c r="L29" s="30" t="s">
+      <c r="K29" s="20"/>
+      <c r="L29" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="M29" s="30" t="s">
+      <c r="M29" s="9" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="180" x14ac:dyDescent="0.25">
-      <c r="A30" s="51">
+      <c r="A30" s="36">
         <v>28</v>
       </c>
-      <c r="B30" s="30" t="s">
+      <c r="B30" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="30" t="s">
+      <c r="C30" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D30" s="30" t="s">
+      <c r="D30" s="9" t="s">
         <v>247</v>
       </c>
-      <c r="E30" s="31">
+      <c r="E30" s="10">
         <v>16</v>
       </c>
-      <c r="F30" s="31"/>
+      <c r="F30" s="10"/>
       <c r="G30" s="21" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="H30" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="I30" s="30" t="s">
+      <c r="I30" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="J30" s="35" t="s">
+      <c r="J30" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="K30" s="35"/>
-      <c r="L30" s="30" t="s">
+      <c r="K30" s="22"/>
+      <c r="L30" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="M30" s="24" t="s">
+      <c r="M30" s="9" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="150" x14ac:dyDescent="0.25">
-      <c r="A31" s="51">
+      <c r="A31" s="36">
         <v>29</v>
       </c>
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C31" s="30" t="s">
+      <c r="C31" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="D31" s="30" t="s">
+      <c r="D31" s="9" t="s">
         <v>248</v>
       </c>
-      <c r="E31" s="31">
+      <c r="E31" s="10">
         <v>16</v>
       </c>
-      <c r="F31" s="31"/>
+      <c r="F31" s="10"/>
       <c r="G31" s="11" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="H31" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="I31" s="30" t="s">
+      <c r="I31" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="J31" s="35" t="s">
+      <c r="J31" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="K31" s="35"/>
-      <c r="L31" s="30" t="s">
+      <c r="K31" s="22"/>
+      <c r="L31" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="M31" s="24" t="s">
+      <c r="M31" s="9" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="165" x14ac:dyDescent="0.25">
-      <c r="A32" s="51">
+      <c r="A32" s="36">
         <v>30</v>
       </c>
-      <c r="B32" s="30" t="s">
+      <c r="B32" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C32" s="30" t="s">
+      <c r="C32" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="D32" s="30" t="s">
+      <c r="D32" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
       <c r="G32" s="21" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="H32" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="I32" s="30" t="s">
+      <c r="I32" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="J32" s="35" t="s">
+      <c r="J32" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="K32" s="36" t="s">
+      <c r="K32" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="L32" s="36" t="s">
+      <c r="L32" s="28" t="s">
         <v>180</v>
       </c>
-      <c r="M32" s="24" t="s">
+      <c r="M32" s="9" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="165" x14ac:dyDescent="0.25">
-      <c r="A33" s="51">
+      <c r="A33" s="36">
         <v>31</v>
       </c>
-      <c r="B33" s="30" t="s">
+      <c r="B33" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="30" t="s">
+      <c r="C33" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="D33" s="30" t="s">
+      <c r="D33" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="E33" s="31"/>
-      <c r="F33" s="31">
+      <c r="E33" s="10"/>
+      <c r="F33" s="10">
         <v>32</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="H33" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="I33" s="30" t="s">
+      <c r="I33" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="J33" s="35" t="s">
+      <c r="J33" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="K33" s="35"/>
-      <c r="L33" s="30" t="s">
+      <c r="K33" s="22"/>
+      <c r="L33" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="M33" s="24" t="s">
+      <c r="M33" s="9" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="135" x14ac:dyDescent="0.25">
-      <c r="A34" s="51">
+      <c r="A34" s="36">
         <v>32</v>
       </c>
-      <c r="B34" s="30" t="s">
+      <c r="B34" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C34" s="30" t="s">
+      <c r="C34" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D34" s="30" t="s">
+      <c r="D34" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31">
+      <c r="E34" s="10"/>
+      <c r="F34" s="10">
         <v>31</v>
       </c>
       <c r="G34" s="11" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="H34" s="11" t="s">
-        <v>358</v>
-      </c>
-      <c r="I34" s="30"/>
-      <c r="J34" s="37" t="s">
+        <v>352</v>
+      </c>
+      <c r="I34" s="9"/>
+      <c r="J34" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="K34" s="32"/>
-      <c r="L34" s="38" t="s">
+      <c r="K34" s="13"/>
+      <c r="L34" s="50" t="s">
         <v>169</v>
       </c>
-      <c r="M34" s="38" t="s">
+      <c r="M34" s="50" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="180" x14ac:dyDescent="0.25">
-      <c r="A35" s="51">
+      <c r="A35" s="36">
         <v>33</v>
       </c>
-      <c r="B35" s="30" t="s">
+      <c r="B35" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C35" s="30" t="s">
+      <c r="C35" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D35" s="30" t="s">
+      <c r="D35" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="E35" s="31">
+      <c r="E35" s="10">
         <v>34</v>
       </c>
-      <c r="F35" s="31"/>
+      <c r="F35" s="10"/>
       <c r="G35" s="11" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="H35" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="I35" s="30"/>
-      <c r="J35" s="30" t="s">
+      <c r="I35" s="9"/>
+      <c r="J35" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="K35" s="32"/>
-      <c r="L35" s="34" t="s">
+      <c r="K35" s="13"/>
+      <c r="L35" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="M35" s="38" t="s">
+      <c r="M35" s="50" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="180" x14ac:dyDescent="0.25">
-      <c r="A36" s="51">
+      <c r="A36" s="36">
         <v>34</v>
       </c>
-      <c r="B36" s="30" t="s">
+      <c r="B36" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C36" s="30" t="s">
+      <c r="C36" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D36" s="30" t="s">
+      <c r="D36" s="9" t="s">
         <v>253</v>
       </c>
-      <c r="E36" s="31"/>
-      <c r="F36" s="31"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
       <c r="G36" s="11" t="s">
         <v>218</v>
       </c>
       <c r="H36" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="I36" s="30"/>
-      <c r="J36" s="30" t="s">
+      <c r="I36" s="9"/>
+      <c r="J36" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="K36" s="32"/>
-      <c r="L36" s="34" t="s">
+      <c r="K36" s="13"/>
+      <c r="L36" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="M36" s="38" t="s">
+      <c r="M36" s="50" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="150" x14ac:dyDescent="0.25">
-      <c r="A37" s="51">
+      <c r="A37" s="36">
         <v>35</v>
       </c>
-      <c r="B37" s="30" t="s">
+      <c r="B37" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C37" s="30" t="s">
+      <c r="C37" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D37" s="30" t="s">
+      <c r="D37" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
       <c r="G37" s="11" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="H37" s="11" t="s">
-        <v>322</v>
-      </c>
-      <c r="I37" s="30"/>
-      <c r="J37" s="37" t="s">
+        <v>316</v>
+      </c>
+      <c r="I37" s="9"/>
+      <c r="J37" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="K37" s="32"/>
-      <c r="L37" s="39" t="s">
+      <c r="K37" s="13"/>
+      <c r="L37" s="51" t="s">
         <v>172</v>
       </c>
-      <c r="M37" s="39" t="s">
+      <c r="M37" s="51" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="150" x14ac:dyDescent="0.25">
-      <c r="A38" s="51">
+      <c r="A38" s="36">
         <v>36</v>
       </c>
-      <c r="B38" s="30" t="s">
+      <c r="B38" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="C38" s="30" t="s">
+      <c r="C38" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D38" s="30" t="s">
+      <c r="D38" s="9" t="s">
         <v>255</v>
       </c>
-      <c r="E38" s="31"/>
-      <c r="F38" s="31"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
       <c r="G38" s="11" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="H38" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="I38" s="30" t="s">
+      <c r="I38" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="J38" s="35" t="s">
+      <c r="J38" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="K38" s="35"/>
-      <c r="L38" s="30" t="s">
+      <c r="K38" s="22"/>
+      <c r="L38" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="M38" s="24" t="s">
+      <c r="M38" s="9" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="180" x14ac:dyDescent="0.25">
-      <c r="A39" s="51">
+      <c r="A39" s="36">
         <v>37</v>
       </c>
-      <c r="B39" s="40" t="s">
+      <c r="B39" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C39" s="40" t="s">
+      <c r="C39" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="D39" s="40" t="s">
+      <c r="D39" s="14" t="s">
         <v>256</v>
       </c>
-      <c r="E39" s="41"/>
-      <c r="F39" s="41"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
       <c r="G39" s="11" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="H39" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="I39" s="40"/>
-      <c r="J39" s="42"/>
-      <c r="K39" s="40" t="s">
+      <c r="I39" s="14"/>
+      <c r="J39" s="16"/>
+      <c r="K39" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="L39" s="43" t="s">
+      <c r="L39" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="M39" s="24" t="s">
+      <c r="M39" s="14" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="180" x14ac:dyDescent="0.25">
-      <c r="A40" s="51">
+      <c r="A40" s="36">
         <v>38</v>
       </c>
-      <c r="B40" s="40" t="s">
+      <c r="B40" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="C40" s="40" t="s">
+      <c r="C40" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="D40" s="40" t="s">
+      <c r="D40" s="14" t="s">
         <v>257</v>
       </c>
-      <c r="E40" s="41"/>
-      <c r="F40" s="41"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
       <c r="G40" s="11" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="H40" s="11" t="s">
-        <v>323</v>
-      </c>
-      <c r="I40" s="40" t="s">
+        <v>317</v>
+      </c>
+      <c r="I40" s="14" t="s">
         <v>198</v>
       </c>
-      <c r="J40" s="44" t="s">
+      <c r="J40" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="K40" s="44" t="s">
+      <c r="K40" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="L40" s="40" t="s">
+      <c r="L40" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="M40" s="24" t="s">
+      <c r="M40" s="14" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="390" x14ac:dyDescent="0.25">
-      <c r="A41" s="51">
+      <c r="A41" s="36">
         <v>39</v>
       </c>
-      <c r="B41" s="40" t="s">
+      <c r="B41" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C41" s="40" t="s">
+      <c r="C41" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="D41" s="40" t="s">
+      <c r="D41" s="14" t="s">
         <v>258</v>
       </c>
-      <c r="E41" s="41"/>
-      <c r="F41" s="41"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
       <c r="G41" s="11" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="H41" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="I41" s="40" t="s">
+      <c r="I41" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="J41" s="40" t="s">
+      <c r="J41" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K41" s="44" t="s">
+      <c r="K41" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="L41" s="40" t="s">
+      <c r="L41" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="M41" s="24" t="s">
+      <c r="M41" s="14" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="210" x14ac:dyDescent="0.25">
-      <c r="A42" s="51">
+      <c r="A42" s="36">
         <v>40</v>
       </c>
-      <c r="B42" s="40" t="s">
+      <c r="B42" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="C42" s="40" t="s">
+      <c r="C42" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="D42" s="40" t="s">
+      <c r="D42" s="14" t="s">
         <v>259</v>
       </c>
-      <c r="E42" s="41">
+      <c r="E42" s="15">
         <v>17</v>
       </c>
-      <c r="F42" s="41"/>
+      <c r="F42" s="15"/>
       <c r="G42" s="11" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="H42" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="I42" s="40" t="s">
+      <c r="I42" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="J42" s="44" t="s">
+      <c r="J42" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="K42" s="44"/>
-      <c r="L42" s="40" t="s">
+      <c r="K42" s="23"/>
+      <c r="L42" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="M42" s="24" t="s">
+      <c r="M42" s="14" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="165" x14ac:dyDescent="0.25">
-      <c r="A43" s="51">
+      <c r="A43" s="36">
         <v>41</v>
       </c>
-      <c r="B43" s="40" t="s">
+      <c r="B43" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="C43" s="40" t="s">
+      <c r="C43" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="D43" s="40" t="s">
+      <c r="D43" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="E43" s="41">
+      <c r="E43" s="15">
         <v>17</v>
       </c>
-      <c r="F43" s="41"/>
+      <c r="F43" s="15"/>
       <c r="G43" s="11" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="H43" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="I43" s="40" t="s">
+      <c r="I43" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="J43" s="44" t="s">
+      <c r="J43" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="K43" s="44"/>
-      <c r="L43" s="40" t="s">
+      <c r="K43" s="23"/>
+      <c r="L43" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="M43" s="24" t="s">
+      <c r="M43" s="14" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="44" spans="1:13" s="1" customFormat="1" ht="180" x14ac:dyDescent="0.25">
-      <c r="A44" s="51">
+      <c r="A44" s="36">
         <v>42</v>
       </c>
-      <c r="B44" s="45" t="s">
+      <c r="B44" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="C44" s="45" t="s">
+      <c r="C44" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="D44" s="45" t="s">
+      <c r="D44" s="30" t="s">
         <v>261</v>
       </c>
-      <c r="E44" s="46"/>
-      <c r="F44" s="46"/>
+      <c r="E44" s="31"/>
+      <c r="F44" s="31"/>
       <c r="G44" s="11" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="H44" s="11" t="s">
-        <v>318</v>
-      </c>
-      <c r="I44" s="45"/>
-      <c r="J44" s="47"/>
-      <c r="K44" s="47"/>
-      <c r="L44" s="48" t="s">
+        <v>312</v>
+      </c>
+      <c r="I44" s="30"/>
+      <c r="J44" s="32"/>
+      <c r="K44" s="32"/>
+      <c r="L44" s="33" t="s">
         <v>164</v>
       </c>
-      <c r="M44" s="45" t="s">
+      <c r="M44" s="30" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="45" spans="1:13" s="1" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="51">
+      <c r="A45" s="36">
         <v>43</v>
       </c>
-      <c r="B45" s="45" t="s">
+      <c r="B45" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="C45" s="45" t="s">
+      <c r="C45" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="D45" s="45" t="s">
+      <c r="D45" s="30" t="s">
         <v>264</v>
       </c>
-      <c r="E45" s="46"/>
-      <c r="F45" s="46" t="s">
-        <v>312</v>
+      <c r="E45" s="31"/>
+      <c r="F45" s="31" t="s">
+        <v>306</v>
       </c>
       <c r="G45" s="11" t="s">
+        <v>386</v>
+      </c>
+      <c r="H45" s="11" t="s">
+        <v>387</v>
+      </c>
+      <c r="I45" s="30"/>
+      <c r="J45" s="32"/>
+      <c r="K45" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="L45" s="33" t="s">
+        <v>165</v>
+      </c>
+      <c r="M45" s="30" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" s="44" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A46" s="41">
+        <v>44</v>
+      </c>
+      <c r="B46" s="41" t="s">
+        <v>265</v>
+      </c>
+      <c r="C46" s="45" t="s">
+        <v>276</v>
+      </c>
+      <c r="D46" s="45" t="s">
+        <v>277</v>
+      </c>
+      <c r="E46" s="43"/>
+      <c r="F46" s="43"/>
+      <c r="G46" s="47" t="s">
+        <v>360</v>
+      </c>
+      <c r="H46" s="47" t="s">
+        <v>361</v>
+      </c>
+      <c r="I46" s="42"/>
+      <c r="J46" s="42"/>
+      <c r="K46" s="42"/>
+      <c r="L46" s="41"/>
+      <c r="M46" s="45" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" s="44" customFormat="1" ht="225" x14ac:dyDescent="0.25">
+      <c r="A47" s="41">
+        <v>45</v>
+      </c>
+      <c r="B47" s="41" t="s">
+        <v>266</v>
+      </c>
+      <c r="C47" s="45" t="s">
+        <v>270</v>
+      </c>
+      <c r="D47" s="45" t="s">
+        <v>271</v>
+      </c>
+      <c r="E47" s="43"/>
+      <c r="F47" s="43"/>
+      <c r="G47" s="47" t="s">
+        <v>362</v>
+      </c>
+      <c r="H47" s="47" t="s">
+        <v>363</v>
+      </c>
+      <c r="I47" s="42"/>
+      <c r="J47" s="42"/>
+      <c r="K47" s="42"/>
+      <c r="L47" s="41"/>
+      <c r="M47" s="45" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" s="44" customFormat="1" ht="270" x14ac:dyDescent="0.25">
+      <c r="A48" s="41">
+        <v>46</v>
+      </c>
+      <c r="B48" s="41" t="s">
+        <v>267</v>
+      </c>
+      <c r="C48" s="45" t="s">
+        <v>272</v>
+      </c>
+      <c r="D48" s="45" t="s">
+        <v>273</v>
+      </c>
+      <c r="E48" s="43"/>
+      <c r="F48" s="43"/>
+      <c r="G48" s="47" t="s">
+        <v>364</v>
+      </c>
+      <c r="H48" s="47" t="s">
+        <v>365</v>
+      </c>
+      <c r="I48" s="42"/>
+      <c r="J48" s="42"/>
+      <c r="K48" s="42"/>
+      <c r="L48" s="41"/>
+      <c r="M48" s="45" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" s="44" customFormat="1" ht="255" x14ac:dyDescent="0.25">
+      <c r="A49" s="41">
+        <v>47</v>
+      </c>
+      <c r="B49" s="41" t="s">
+        <v>268</v>
+      </c>
+      <c r="C49" s="45" t="s">
+        <v>274</v>
+      </c>
+      <c r="D49" s="45" t="s">
+        <v>275</v>
+      </c>
+      <c r="E49" s="43"/>
+      <c r="F49" s="43"/>
+      <c r="G49" s="47" t="s">
+        <v>366</v>
+      </c>
+      <c r="H49" s="47" t="s">
+        <v>367</v>
+      </c>
+      <c r="I49" s="42"/>
+      <c r="J49" s="42"/>
+      <c r="K49" s="42"/>
+      <c r="L49" s="41"/>
+      <c r="M49" s="45" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" s="44" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A50" s="41">
+        <v>48</v>
+      </c>
+      <c r="B50" s="41" t="s">
+        <v>269</v>
+      </c>
+      <c r="C50" s="45" t="s">
+        <v>278</v>
+      </c>
+      <c r="D50" s="45" t="s">
+        <v>285</v>
+      </c>
+      <c r="E50" s="43"/>
+      <c r="F50" s="43"/>
+      <c r="G50" s="47" t="s">
+        <v>368</v>
+      </c>
+      <c r="H50" s="47" t="s">
+        <v>369</v>
+      </c>
+      <c r="I50" s="42"/>
+      <c r="J50" s="42"/>
+      <c r="K50" s="42"/>
+      <c r="L50" s="41"/>
+      <c r="M50" s="48" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" s="44" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A51" s="41">
+        <v>49</v>
+      </c>
+      <c r="B51" s="45" t="s">
+        <v>388</v>
+      </c>
+      <c r="C51" s="45" t="s">
+        <v>279</v>
+      </c>
+      <c r="D51" s="45" t="s">
+        <v>280</v>
+      </c>
+      <c r="E51" s="43"/>
+      <c r="F51" s="43"/>
+      <c r="G51" s="47" t="s">
+        <v>370</v>
+      </c>
+      <c r="H51" s="47" t="s">
+        <v>371</v>
+      </c>
+      <c r="I51" s="42"/>
+      <c r="J51" s="42"/>
+      <c r="K51" s="42"/>
+      <c r="L51" s="41"/>
+      <c r="M51" s="45" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" s="44" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A52" s="41">
+        <v>60</v>
+      </c>
+      <c r="B52" s="45" t="s">
+        <v>389</v>
+      </c>
+      <c r="C52" s="45" t="s">
+        <v>282</v>
+      </c>
+      <c r="D52" s="45" t="s">
+        <v>281</v>
+      </c>
+      <c r="E52" s="43"/>
+      <c r="F52" s="43"/>
+      <c r="G52" s="47" t="s">
+        <v>372</v>
+      </c>
+      <c r="H52" s="47" t="s">
+        <v>373</v>
+      </c>
+      <c r="I52" s="42"/>
+      <c r="J52" s="42"/>
+      <c r="K52" s="42"/>
+      <c r="L52" s="41"/>
+      <c r="M52" s="45" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" s="44" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A53" s="41">
+        <v>51</v>
+      </c>
+      <c r="B53" s="41" t="s">
+        <v>390</v>
+      </c>
+      <c r="C53" s="45" t="s">
+        <v>391</v>
+      </c>
+      <c r="D53" s="45" t="s">
         <v>392</v>
       </c>
-      <c r="H45" s="11" t="s">
+      <c r="E53" s="43"/>
+      <c r="F53" s="43"/>
+      <c r="G53" s="47" t="s">
+        <v>374</v>
+      </c>
+      <c r="H53" s="47" t="s">
+        <v>375</v>
+      </c>
+      <c r="I53" s="42"/>
+      <c r="J53" s="42"/>
+      <c r="K53" s="42"/>
+      <c r="L53" s="41"/>
+      <c r="M53" s="48" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" s="44" customFormat="1" ht="210" x14ac:dyDescent="0.25">
+      <c r="A54" s="41">
+        <v>52</v>
+      </c>
+      <c r="B54" s="45" t="s">
         <v>393</v>
       </c>
-      <c r="I45" s="45"/>
-      <c r="J45" s="47"/>
-      <c r="K45" s="49" t="s">
-        <v>29</v>
-      </c>
-      <c r="L45" s="48" t="s">
-        <v>165</v>
-      </c>
-      <c r="M45" s="45" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" s="59" customFormat="1" ht="180" x14ac:dyDescent="0.25">
-      <c r="A46" s="56">
-        <v>44</v>
-      </c>
-      <c r="B46" s="56" t="s">
-        <v>265</v>
-      </c>
-      <c r="C46" s="60" t="s">
-        <v>280</v>
-      </c>
-      <c r="D46" s="60" t="s">
-        <v>281</v>
-      </c>
-      <c r="E46" s="58"/>
-      <c r="F46" s="58"/>
-      <c r="G46" s="62" t="s">
-        <v>366</v>
-      </c>
-      <c r="H46" s="62" t="s">
-        <v>367</v>
-      </c>
-      <c r="I46" s="57"/>
-      <c r="J46" s="57"/>
-      <c r="K46" s="57"/>
-      <c r="L46" s="56"/>
-      <c r="M46" s="60" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" s="59" customFormat="1" ht="225" x14ac:dyDescent="0.25">
-      <c r="A47" s="56">
-        <v>45</v>
-      </c>
-      <c r="B47" s="56" t="s">
-        <v>266</v>
-      </c>
-      <c r="C47" s="60" t="s">
-        <v>274</v>
-      </c>
-      <c r="D47" s="60" t="s">
-        <v>275</v>
-      </c>
-      <c r="E47" s="58"/>
-      <c r="F47" s="58"/>
-      <c r="G47" s="62" t="s">
-        <v>368</v>
-      </c>
-      <c r="H47" s="62" t="s">
-        <v>369</v>
-      </c>
-      <c r="I47" s="57"/>
-      <c r="J47" s="57"/>
-      <c r="K47" s="57"/>
-      <c r="L47" s="56"/>
-      <c r="M47" s="60" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" s="59" customFormat="1" ht="270" x14ac:dyDescent="0.25">
-      <c r="A48" s="56">
-        <v>46</v>
-      </c>
-      <c r="B48" s="56" t="s">
-        <v>267</v>
-      </c>
-      <c r="C48" s="60" t="s">
-        <v>276</v>
-      </c>
-      <c r="D48" s="60" t="s">
-        <v>277</v>
-      </c>
-      <c r="E48" s="58"/>
-      <c r="F48" s="58"/>
-      <c r="G48" s="62" t="s">
-        <v>370</v>
-      </c>
-      <c r="H48" s="62" t="s">
-        <v>371</v>
-      </c>
-      <c r="I48" s="57"/>
-      <c r="J48" s="57"/>
-      <c r="K48" s="57"/>
-      <c r="L48" s="56"/>
-      <c r="M48" s="60" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" s="59" customFormat="1" ht="255" x14ac:dyDescent="0.25">
-      <c r="A49" s="56">
-        <v>47</v>
-      </c>
-      <c r="B49" s="56" t="s">
-        <v>268</v>
-      </c>
-      <c r="C49" s="60" t="s">
-        <v>278</v>
-      </c>
-      <c r="D49" s="60" t="s">
-        <v>279</v>
-      </c>
-      <c r="E49" s="58"/>
-      <c r="F49" s="58"/>
-      <c r="G49" s="62" t="s">
-        <v>372</v>
-      </c>
-      <c r="H49" s="62" t="s">
-        <v>373</v>
-      </c>
-      <c r="I49" s="57"/>
-      <c r="J49" s="57"/>
-      <c r="K49" s="57"/>
-      <c r="L49" s="56"/>
-      <c r="M49" s="60" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" s="59" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A50" s="56">
-        <v>48</v>
-      </c>
-      <c r="B50" s="56" t="s">
-        <v>269</v>
-      </c>
-      <c r="C50" s="60" t="s">
-        <v>282</v>
-      </c>
-      <c r="D50" s="60" t="s">
-        <v>289</v>
-      </c>
-      <c r="E50" s="58"/>
-      <c r="F50" s="58"/>
-      <c r="G50" s="62" t="s">
-        <v>374</v>
-      </c>
-      <c r="H50" s="62" t="s">
-        <v>375</v>
-      </c>
-      <c r="I50" s="57"/>
-      <c r="J50" s="57"/>
-      <c r="K50" s="57"/>
-      <c r="L50" s="56"/>
-      <c r="M50" s="63" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" s="59" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A51" s="56">
-        <v>49</v>
-      </c>
-      <c r="B51" s="56" t="s">
-        <v>270</v>
-      </c>
-      <c r="C51" s="60" t="s">
+      <c r="C54" s="45" t="s">
         <v>283</v>
       </c>
-      <c r="D51" s="60" t="s">
+      <c r="D54" s="45" t="s">
         <v>284</v>
       </c>
-      <c r="E51" s="58"/>
-      <c r="F51" s="58"/>
-      <c r="G51" s="62" t="s">
+      <c r="E54" s="43"/>
+      <c r="F54" s="43"/>
+      <c r="G54" s="47" t="s">
         <v>376</v>
       </c>
-      <c r="H51" s="62" t="s">
+      <c r="H54" s="47" t="s">
         <v>377</v>
       </c>
-      <c r="I51" s="57"/>
-      <c r="J51" s="57"/>
-      <c r="K51" s="57"/>
-      <c r="L51" s="56"/>
-      <c r="M51" s="60" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" s="59" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A52" s="56">
-        <v>60</v>
-      </c>
-      <c r="B52" s="56" t="s">
-        <v>271</v>
-      </c>
-      <c r="C52" s="60" t="s">
-        <v>286</v>
-      </c>
-      <c r="D52" s="60" t="s">
-        <v>285</v>
-      </c>
-      <c r="E52" s="58"/>
-      <c r="F52" s="58"/>
-      <c r="G52" s="62" t="s">
-        <v>378</v>
-      </c>
-      <c r="H52" s="62" t="s">
-        <v>379</v>
-      </c>
-      <c r="I52" s="57"/>
-      <c r="J52" s="57"/>
-      <c r="K52" s="57"/>
-      <c r="L52" s="56"/>
-      <c r="M52" s="60" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" s="59" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A53" s="56">
-        <v>51</v>
-      </c>
-      <c r="B53" s="56" t="s">
-        <v>273</v>
-      </c>
-      <c r="C53" s="60" t="s">
-        <v>298</v>
-      </c>
-      <c r="D53" s="60" t="s">
-        <v>299</v>
-      </c>
-      <c r="E53" s="58"/>
-      <c r="F53" s="58"/>
-      <c r="G53" s="62" t="s">
-        <v>380</v>
-      </c>
-      <c r="H53" s="62" t="s">
-        <v>381</v>
-      </c>
-      <c r="I53" s="57"/>
-      <c r="J53" s="57"/>
-      <c r="K53" s="57"/>
-      <c r="L53" s="56"/>
-      <c r="M53" s="63" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" s="59" customFormat="1" ht="210" x14ac:dyDescent="0.25">
-      <c r="A54" s="56">
-        <v>52</v>
-      </c>
-      <c r="B54" s="56" t="s">
-        <v>272</v>
-      </c>
-      <c r="C54" s="60" t="s">
+      <c r="I54" s="42"/>
+      <c r="J54" s="42"/>
+      <c r="K54" s="42"/>
+      <c r="L54" s="41"/>
+      <c r="M54" s="45" t="s">
         <v>287</v>
-      </c>
-      <c r="D54" s="60" t="s">
-        <v>288</v>
-      </c>
-      <c r="E54" s="58"/>
-      <c r="F54" s="58"/>
-      <c r="G54" s="62" t="s">
-        <v>382</v>
-      </c>
-      <c r="H54" s="62" t="s">
-        <v>383</v>
-      </c>
-      <c r="I54" s="57"/>
-      <c r="J54" s="57"/>
-      <c r="K54" s="57"/>
-      <c r="L54" s="56"/>
-      <c r="M54" s="60" t="s">
-        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -4512,7 +4469,7 @@
     </row>
     <row r="7" spans="1:1" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="60" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
was missing link in one activity
</commit_message>
<xml_diff>
--- a/actions/Activities.xlsx
+++ b/actions/Activities.xlsx
@@ -1792,9 +1792,6 @@
     <t>Adopting the right mindset is crucial in altering one's behavior (e.g., quitting smoking). It involves identifying the desired end result and having faith in one's ability to attain it. Adequate motivation and self-confidence are crucial in this process. To understand why, I recommend watching the short video that I will send you in a message on Prolific right after this session. What do you think, how can self-confidence and motivation help you to reach your end goal? Write down your thoughts on a piece of paper or your phone.</t>
   </si>
   <si>
-    <t>Adopting the right mindset is crucial in altering one's behavior (e.g., quitting smoking). It involves identifying the desired end result and having faith in one's ability to attain it. Adequate motivation and self-confidence are crucial in this process. To understand why, I recommend watching this short video before the next session: &lt;insert our link&gt;. What do you think, how can self-confidence and motivation help you to reach your end goal? Write down your thoughts on a piece of paper or your phone.</t>
-  </si>
-  <si>
     <t>Some very practical steps can aid in effectively changing your behavior (e.g., quitting smoking). This includes acquiring an understanding of your current behavior, exploring strategies to overcome possible obstacles, and preparing things that will motivate you. To understand why, I advise watching the short video that I will send you in a message on Prolific right after this session. How do you think practical preparations can help you become more physically active and quit smoking? Write down your thoughts on a piece of paper or your phone.</t>
   </si>
   <si>
@@ -1892,6 +1889,9 @@
   </si>
   <si>
     <t>learn about how thinking of possible obstacles is useful to succeed in changing your behavior</t>
+  </si>
+  <si>
+    <t>Adopting the right mindset is crucial in altering one's behavior (e.g., quitting smoking). It involves identifying the desired end result and having faith in one's ability to attain it. Adequate motivation and self-confidence are crucial in this process. To understand why, I recommend watching this short video before the next session: https://youtu.be/CAQ_P4Z7z4Q. What do you think, how can self-confidence and motivation help you to reach your end goal? Write down your thoughts on a piece of paper or your phone.</t>
   </si>
 </sst>
 </file>
@@ -2472,10 +2472,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="F53" sqref="F53"/>
+      <selection pane="bottomLeft" activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2501,7 +2501,7 @@
         <v>128</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D1" s="43" t="s">
         <v>129</v>
@@ -2944,10 +2944,10 @@
         <v>11</v>
       </c>
       <c r="H12" s="8" t="s">
+        <v>361</v>
+      </c>
+      <c r="I12" s="8" t="s">
         <v>362</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>363</v>
       </c>
       <c r="J12" s="6"/>
       <c r="K12" s="9"/>
@@ -2984,10 +2984,10 @@
         <v>10</v>
       </c>
       <c r="H13" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="I13" s="8" t="s">
         <v>364</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>365</v>
       </c>
       <c r="J13" s="11"/>
       <c r="K13" s="13"/>
@@ -3020,10 +3020,10 @@
         <v>289</v>
       </c>
       <c r="H14" s="8" t="s">
+        <v>365</v>
+      </c>
+      <c r="I14" s="8" t="s">
         <v>366</v>
-      </c>
-      <c r="I14" s="8" t="s">
-        <v>367</v>
       </c>
       <c r="J14" s="6"/>
       <c r="K14" s="9"/>
@@ -3058,10 +3058,10 @@
         <v>290</v>
       </c>
       <c r="H15" s="8" t="s">
+        <v>367</v>
+      </c>
+      <c r="I15" s="8" t="s">
         <v>368</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>369</v>
       </c>
       <c r="J15" s="11"/>
       <c r="K15" s="13"/>
@@ -4214,10 +4214,10 @@
         <v>291</v>
       </c>
       <c r="H45" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="I45" s="8" t="s">
         <v>370</v>
-      </c>
-      <c r="I45" s="8" t="s">
-        <v>371</v>
       </c>
       <c r="J45" s="27"/>
       <c r="K45" s="29"/>
@@ -4253,7 +4253,7 @@
         <v>344</v>
       </c>
       <c r="I46" s="44" t="s">
-        <v>345</v>
+        <v>378</v>
       </c>
       <c r="J46" s="39"/>
       <c r="K46" s="39"/>
@@ -4282,10 +4282,10 @@
       <c r="F47" s="40"/>
       <c r="G47" s="40"/>
       <c r="H47" s="44" t="s">
+        <v>345</v>
+      </c>
+      <c r="I47" s="44" t="s">
         <v>346</v>
-      </c>
-      <c r="I47" s="44" t="s">
-        <v>347</v>
       </c>
       <c r="J47" s="39"/>
       <c r="K47" s="39"/>
@@ -4314,10 +4314,10 @@
       <c r="F48" s="40"/>
       <c r="G48" s="40"/>
       <c r="H48" s="44" t="s">
+        <v>347</v>
+      </c>
+      <c r="I48" s="44" t="s">
         <v>348</v>
-      </c>
-      <c r="I48" s="44" t="s">
-        <v>349</v>
       </c>
       <c r="J48" s="39"/>
       <c r="K48" s="39"/>
@@ -4346,10 +4346,10 @@
       <c r="F49" s="40"/>
       <c r="G49" s="40"/>
       <c r="H49" s="44" t="s">
+        <v>349</v>
+      </c>
+      <c r="I49" s="44" t="s">
         <v>350</v>
-      </c>
-      <c r="I49" s="44" t="s">
-        <v>351</v>
       </c>
       <c r="J49" s="39"/>
       <c r="K49" s="39"/>
@@ -4378,10 +4378,10 @@
       <c r="F50" s="40"/>
       <c r="G50" s="40"/>
       <c r="H50" s="44" t="s">
+        <v>351</v>
+      </c>
+      <c r="I50" s="44" t="s">
         <v>352</v>
-      </c>
-      <c r="I50" s="44" t="s">
-        <v>353</v>
       </c>
       <c r="J50" s="39"/>
       <c r="K50" s="39"/>
@@ -4396,7 +4396,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="42" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C51" s="51">
         <v>11</v>
@@ -4410,10 +4410,10 @@
       <c r="F51" s="40"/>
       <c r="G51" s="40"/>
       <c r="H51" s="44" t="s">
+        <v>353</v>
+      </c>
+      <c r="I51" s="44" t="s">
         <v>354</v>
-      </c>
-      <c r="I51" s="44" t="s">
-        <v>355</v>
       </c>
       <c r="J51" s="39"/>
       <c r="K51" s="39"/>
@@ -4428,7 +4428,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="42" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C52" s="51">
         <v>12</v>
@@ -4442,10 +4442,10 @@
       <c r="F52" s="40"/>
       <c r="G52" s="40"/>
       <c r="H52" s="44" t="s">
+        <v>355</v>
+      </c>
+      <c r="I52" s="44" t="s">
         <v>356</v>
-      </c>
-      <c r="I52" s="44" t="s">
-        <v>357</v>
       </c>
       <c r="J52" s="39"/>
       <c r="K52" s="39"/>
@@ -4460,24 +4460,24 @@
         <v>51</v>
       </c>
       <c r="B53" s="38" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C53" s="40">
         <v>13</v>
       </c>
       <c r="D53" s="42" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E53" s="42" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F53" s="40"/>
       <c r="G53" s="40"/>
       <c r="H53" s="44" t="s">
+        <v>357</v>
+      </c>
+      <c r="I53" s="44" t="s">
         <v>358</v>
-      </c>
-      <c r="I53" s="44" t="s">
-        <v>359</v>
       </c>
       <c r="J53" s="39"/>
       <c r="K53" s="39"/>
@@ -4492,7 +4492,7 @@
         <v>52</v>
       </c>
       <c r="B54" s="42" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C54" s="51">
         <v>14</v>
@@ -4506,10 +4506,10 @@
       <c r="F54" s="40"/>
       <c r="G54" s="40"/>
       <c r="H54" s="44" t="s">
+        <v>359</v>
+      </c>
+      <c r="I54" s="44" t="s">
         <v>360</v>
-      </c>
-      <c r="I54" s="44" t="s">
-        <v>361</v>
       </c>
       <c r="J54" s="39"/>
       <c r="K54" s="39"/>

</xml_diff>

<commit_message>
typos in activity titles
</commit_message>
<xml_diff>
--- a/actions/Activities.xlsx
+++ b/actions/Activities.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nalbers1\Documents\Exp1\virtual_coach_useful_activities\actions\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAAA41BF-17CE-40CC-86E1-547840B6BAEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-120" windowWidth="19200" windowHeight="5520"/>
+    <workbookView xWindow="-19310" yWindow="0" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="6" r:id="rId1"/>
@@ -19,15 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -175,9 +167,6 @@
     <t>Thinking of routines that cause cravings to smoke and how to change them to reduce or avoid cravings.</t>
   </si>
   <si>
-    <t>Thinking of high risk situations and how to cope with them</t>
-  </si>
-  <si>
     <t>Progressive muscle relaxation</t>
   </si>
   <si>
@@ -244,9 +233,6 @@
     <t>E.g. this video: https://www.youtube.com/watch?v=GHZXsvrL270</t>
   </si>
   <si>
-    <t>Education on the relationsip between stress and smoking</t>
-  </si>
-  <si>
     <t>e.g. this video: https://www.youtube.com/watch?v=nysjq8VIwI8&amp;ab_channel=EveryMindMatters</t>
   </si>
   <si>
@@ -350,12 +336,6 @@
   </si>
   <si>
     <t>Education on diet</t>
-  </si>
-  <si>
-    <t>How friends and/or family will receive one's desired futrue self after quitting smoking</t>
-  </si>
-  <si>
-    <t>How friends and/or family will receive one's desired futrue self after becoming more physically active</t>
   </si>
   <si>
     <t>Envisioning and writing down how one's family and/or friends will receive one's desired future self after quitting smoking.</t>
@@ -1893,11 +1873,23 @@
   <si>
     <t>Adopting the right mindset is crucial in altering one's behavior (e.g., quitting smoking). It involves identifying the desired end result and having faith in one's ability to attain it. Adequate motivation and self-confidence are crucial in this process. To understand why, I recommend watching this short video before the next session: https://youtu.be/CAQ_P4Z7z4Q. What do you think, how can self-confidence and motivation help you to reach your end goal? Write down your thoughts on a piece of paper or your phone.</t>
   </si>
+  <si>
+    <t>Education on the relationship between stress and smoking</t>
+  </si>
+  <si>
+    <t>Thinking of high-risk situations and how to cope with them</t>
+  </si>
+  <si>
+    <t>How friends and/or family will receive one's desired future self after quitting smoking</t>
+  </si>
+  <si>
+    <t>How friends and/or family will receive one's desired future self after becoming more physically active</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2469,13 +2461,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="I46" sqref="I46"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2495,46 +2487,46 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="D1" s="43" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1" s="43" t="s">
+        <v>209</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>283</v>
+      </c>
+      <c r="I1" s="34" t="s">
+        <v>284</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="D1" s="43" t="s">
-        <v>129</v>
-      </c>
-      <c r="E1" s="43" t="s">
-        <v>213</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="H1" s="36" t="s">
-        <v>287</v>
-      </c>
-      <c r="I1" s="34" t="s">
-        <v>288</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>132</v>
-      </c>
       <c r="N1" s="43" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="105" x14ac:dyDescent="0.25">
@@ -2542,26 +2534,26 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C2" s="32">
         <v>5</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7">
         <v>1</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="J2" s="6"/>
       <c r="K2" s="9"/>
@@ -2578,26 +2570,26 @@
         <v>1</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C3" s="32">
         <v>5</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="F3" s="12"/>
       <c r="G3" s="12">
         <v>0</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="J3" s="11"/>
       <c r="K3" s="13"/>
@@ -2614,37 +2606,37 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C4" s="32">
         <v>4</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7">
         <v>3</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="J4" s="6"/>
       <c r="K4" s="15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L4" s="16"/>
       <c r="M4" s="17" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="N4" s="17" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="150" x14ac:dyDescent="0.25">
@@ -2652,35 +2644,35 @@
         <v>3</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C5" s="32">
         <v>4</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="F5" s="12"/>
       <c r="G5" s="12">
         <v>2</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="J5" s="11"/>
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
       <c r="M5" s="11" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="N5" s="11" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="210" x14ac:dyDescent="0.25">
@@ -2694,33 +2686,33 @@
         <v>5</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7">
         <v>24</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="I6" s="18" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="J6" s="19" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="K6" s="19" t="s">
         <v>0</v>
       </c>
       <c r="L6" s="19"/>
       <c r="M6" s="6" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="210" x14ac:dyDescent="0.25">
@@ -2728,39 +2720,39 @@
         <v>5</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C7" s="32">
         <v>5</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="12">
         <v>25</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="I7" s="18" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="K7" s="20" t="s">
         <v>16</v>
       </c>
       <c r="L7" s="20"/>
       <c r="M7" s="11" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="N7" s="11" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="195" x14ac:dyDescent="0.25">
@@ -2777,18 +2769,18 @@
         <v>37</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="8" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="K8" s="19" t="s">
         <v>1</v>
@@ -2797,10 +2789,10 @@
         <v>34</v>
       </c>
       <c r="M8" s="10" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="N8" s="21" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="150" x14ac:dyDescent="0.25">
@@ -2808,37 +2800,37 @@
         <v>7</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C9" s="32">
         <v>4</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
       <c r="H9" s="18" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="I9" s="18" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="K9" s="20" t="s">
         <v>14</v>
       </c>
       <c r="L9" s="20"/>
       <c r="M9" s="11" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="N9" s="21" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="150" x14ac:dyDescent="0.25">
@@ -2846,39 +2838,39 @@
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C10" s="32">
         <v>4</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7">
         <v>9</v>
       </c>
       <c r="H10" s="18" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="I10" s="18" t="s">
         <v>9</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="K10" s="19" t="s">
         <v>9</v>
       </c>
       <c r="L10" s="19"/>
       <c r="M10" s="6" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="N10" s="21" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="195" x14ac:dyDescent="0.25">
@@ -2886,39 +2878,39 @@
         <v>9</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C11" s="32">
         <v>4</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="F11" s="12"/>
       <c r="G11" s="12">
         <v>8</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="K11" s="20" t="s">
         <v>23</v>
       </c>
       <c r="L11" s="20"/>
       <c r="M11" s="11" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="N11" s="21" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="225" x14ac:dyDescent="0.25">
@@ -2926,28 +2918,28 @@
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>102</v>
+        <v>377</v>
       </c>
       <c r="C12" s="32">
         <v>5</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="G12" s="7">
         <v>11</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="J12" s="6"/>
       <c r="K12" s="9"/>
@@ -2955,10 +2947,10 @@
         <v>24</v>
       </c>
       <c r="M12" s="6" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="N12" s="21" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="240" x14ac:dyDescent="0.25">
@@ -2966,37 +2958,37 @@
         <v>11</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>103</v>
+        <v>378</v>
       </c>
       <c r="C13" s="32">
         <v>5</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="G13" s="12">
         <v>10</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="J13" s="11"/>
       <c r="K13" s="13"/>
       <c r="L13" s="14"/>
       <c r="M13" s="11" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="N13" s="21" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="210" x14ac:dyDescent="0.25">
@@ -3004,37 +2996,37 @@
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C14" s="32">
         <v>4</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="J14" s="6"/>
       <c r="K14" s="9"/>
       <c r="L14" s="22" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="M14" s="17" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="N14" s="6" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="180" x14ac:dyDescent="0.25">
@@ -3042,37 +3034,37 @@
         <v>13</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C15" s="32">
         <v>4</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="F15" s="12"/>
       <c r="G15" s="12" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="J15" s="11"/>
       <c r="K15" s="13"/>
       <c r="L15" s="23" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="M15" s="24" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="N15" s="11" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="225" x14ac:dyDescent="0.25">
@@ -3080,26 +3072,26 @@
         <v>14</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C16" s="32">
         <v>5</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7">
         <v>15</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="J16" s="6"/>
       <c r="K16" s="9"/>
@@ -3107,10 +3099,10 @@
         <v>31</v>
       </c>
       <c r="M16" s="25" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="N16" s="21" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="135" x14ac:dyDescent="0.25">
@@ -3118,35 +3110,35 @@
         <v>15</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C17" s="32">
         <v>5</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="F17" s="12"/>
       <c r="G17" s="12">
         <v>14</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="J17" s="11"/>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
       <c r="M17" s="26" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="N17" s="21" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="150" x14ac:dyDescent="0.25">
@@ -3154,37 +3146,37 @@
         <v>16</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C18" s="32">
         <v>3</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="8" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="I18" s="8" t="s">
         <v>11</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="K18" s="19" t="s">
         <v>11</v>
       </c>
       <c r="L18" s="19"/>
       <c r="M18" s="6" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="N18" s="21" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="210" x14ac:dyDescent="0.25">
@@ -3192,37 +3184,37 @@
         <v>17</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C19" s="32">
         <v>3</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="F19" s="12"/>
       <c r="G19" s="12"/>
       <c r="H19" s="8" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="J19" s="11" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="K19" s="20" t="s">
         <v>12</v>
       </c>
       <c r="L19" s="20"/>
       <c r="M19" s="11" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="N19" s="21" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="150" x14ac:dyDescent="0.25">
@@ -3236,33 +3228,33 @@
         <v>1</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="7">
         <v>20</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="K20" s="19" t="s">
         <v>2</v>
       </c>
       <c r="L20" s="19"/>
       <c r="M20" s="6" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="N20" s="21" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="210" x14ac:dyDescent="0.25">
@@ -3270,39 +3262,39 @@
         <v>19</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" s="32">
         <v>1</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="F21" s="12"/>
       <c r="G21" s="12">
         <v>21</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J21" s="11" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="K21" s="20" t="s">
         <v>17</v>
       </c>
       <c r="L21" s="20"/>
       <c r="M21" s="11" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="N21" s="21" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="210" x14ac:dyDescent="0.25">
@@ -3316,33 +3308,33 @@
         <v>1</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="7">
         <v>18</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="K22" s="19" t="s">
         <v>3</v>
       </c>
       <c r="L22" s="19"/>
       <c r="M22" s="6" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="N22" s="21" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="225" x14ac:dyDescent="0.25">
@@ -3350,39 +3342,39 @@
         <v>21</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C23" s="32">
         <v>1</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="F23" s="12"/>
       <c r="G23" s="12">
         <v>19</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="J23" s="11" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="K23" s="20" t="s">
         <v>18</v>
       </c>
       <c r="L23" s="20"/>
       <c r="M23" s="11" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="N23" s="21" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="150" x14ac:dyDescent="0.25">
@@ -3390,39 +3382,39 @@
         <v>22</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C24" s="32">
         <v>5</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="7">
         <v>23</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="K24" s="19" t="s">
         <v>4</v>
       </c>
       <c r="L24" s="19"/>
       <c r="M24" s="6" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="N24" s="21" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="180" x14ac:dyDescent="0.25">
@@ -3430,39 +3422,39 @@
         <v>23</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C25" s="32">
         <v>5</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="F25" s="12"/>
       <c r="G25" s="12">
         <v>22</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="J25" s="11" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="K25" s="20" t="s">
         <v>19</v>
       </c>
       <c r="L25" s="20"/>
       <c r="M25" s="11" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="N25" s="21" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="210" x14ac:dyDescent="0.25">
@@ -3470,37 +3462,37 @@
         <v>24</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C26" s="32">
         <v>5</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="7">
         <v>4</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="I26" s="18" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="K26" s="9"/>
       <c r="L26" s="9"/>
       <c r="M26" s="6" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="N26" s="21" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="210" x14ac:dyDescent="0.25">
@@ -3508,39 +3500,39 @@
         <v>25</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C27" s="32">
         <v>5</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="F27" s="12"/>
       <c r="G27" s="12">
         <v>5</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="J27" s="11" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="K27" s="20" t="s">
         <v>20</v>
       </c>
       <c r="L27" s="20"/>
       <c r="M27" s="11" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="N27" s="21" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="225" x14ac:dyDescent="0.25">
@@ -3554,31 +3546,31 @@
         <v>2</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
       <c r="H28" s="8" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="J28" s="6"/>
       <c r="K28" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L28" s="10" t="s">
         <v>33</v>
       </c>
       <c r="M28" s="46" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="N28" s="6" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="135" x14ac:dyDescent="0.25">
@@ -3586,35 +3578,35 @@
         <v>27</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>66</v>
+        <v>375</v>
       </c>
       <c r="C29" s="32">
         <v>2</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
       <c r="H29" s="8" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="J29" s="6"/>
       <c r="K29" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L29" s="17"/>
       <c r="M29" s="6" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="N29" s="6" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="180" x14ac:dyDescent="0.25">
@@ -3631,30 +3623,30 @@
         <v>42</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="F30" s="7">
         <v>16</v>
       </c>
       <c r="G30" s="7"/>
       <c r="H30" s="18" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="I30" s="18" t="s">
         <v>5</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="K30" s="19" t="s">
         <v>5</v>
       </c>
       <c r="L30" s="19"/>
       <c r="M30" s="6" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="N30" s="6" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="150" x14ac:dyDescent="0.25">
@@ -3662,39 +3654,39 @@
         <v>29</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>43</v>
+        <v>376</v>
       </c>
       <c r="C31" s="32">
         <v>3</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F31" s="7">
         <v>16</v>
       </c>
       <c r="G31" s="7"/>
       <c r="H31" s="8" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="K31" s="19" t="s">
         <v>6</v>
       </c>
       <c r="L31" s="19"/>
       <c r="M31" s="6" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="N31" s="6" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="165" x14ac:dyDescent="0.25">
@@ -3702,27 +3694,27 @@
         <v>30</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C32" s="32">
         <v>3</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="7"/>
       <c r="H32" s="18" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="I32" s="18" t="s">
         <v>7</v>
       </c>
       <c r="J32" s="6" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="K32" s="19" t="s">
         <v>7</v>
@@ -3731,10 +3723,10 @@
         <v>27</v>
       </c>
       <c r="M32" s="25" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="N32" s="6" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="165" x14ac:dyDescent="0.25">
@@ -3742,39 +3734,39 @@
         <v>31</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C33" s="32">
         <v>2</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="F33" s="7"/>
       <c r="G33" s="7">
         <v>32</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="K33" s="19" t="s">
         <v>8</v>
       </c>
       <c r="L33" s="19"/>
       <c r="M33" s="6" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="N33" s="6" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="135" x14ac:dyDescent="0.25">
@@ -3788,31 +3780,31 @@
         <v>2</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="F34" s="7"/>
       <c r="G34" s="7">
         <v>31</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="J34" s="6"/>
       <c r="K34" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L34" s="10"/>
       <c r="M34" s="47" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="N34" s="47" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="180" x14ac:dyDescent="0.25">
@@ -3820,37 +3812,37 @@
         <v>33</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C35" s="32">
         <v>2</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="F35" s="7">
         <v>34</v>
       </c>
       <c r="G35" s="7"/>
       <c r="H35" s="8" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J35" s="6"/>
       <c r="K35" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L35" s="10"/>
       <c r="M35" s="17" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="N35" s="47" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="180" x14ac:dyDescent="0.25">
@@ -3858,35 +3850,35 @@
         <v>34</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C36" s="32">
         <v>2</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
       <c r="H36" s="8" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="J36" s="6"/>
       <c r="K36" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L36" s="10"/>
       <c r="M36" s="17" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="N36" s="47" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="150" x14ac:dyDescent="0.25">
@@ -3894,35 +3886,35 @@
         <v>35</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C37" s="32">
         <v>2</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
       <c r="H37" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="I37" s="8" t="s">
         <v>296</v>
-      </c>
-      <c r="I37" s="8" t="s">
-        <v>300</v>
       </c>
       <c r="J37" s="6"/>
       <c r="K37" s="15" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="L37" s="10"/>
       <c r="M37" s="48" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="N37" s="48" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="150" x14ac:dyDescent="0.25">
@@ -3930,37 +3922,37 @@
         <v>36</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C38" s="32">
         <v>4</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="F38" s="7"/>
       <c r="G38" s="7"/>
       <c r="H38" s="8" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="K38" s="19" t="s">
         <v>10</v>
       </c>
       <c r="L38" s="19"/>
       <c r="M38" s="6" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="N38" s="6" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="180" x14ac:dyDescent="0.25">
@@ -3968,24 +3960,24 @@
         <v>37</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C39" s="32">
         <v>3</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="F39" s="12"/>
       <c r="G39" s="12"/>
       <c r="H39" s="8" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="J39" s="11"/>
       <c r="K39" s="13"/>
@@ -3996,7 +3988,7 @@
         <v>26</v>
       </c>
       <c r="N39" s="11" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="180" x14ac:dyDescent="0.25">
@@ -4004,39 +3996,39 @@
         <v>38</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C40" s="32">
         <v>3</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F40" s="12"/>
       <c r="G40" s="12"/>
       <c r="H40" s="8" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="J40" s="11" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="K40" s="20" t="s">
         <v>22</v>
       </c>
       <c r="L40" s="20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="M40" s="11" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="N40" s="11" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="390" x14ac:dyDescent="0.25">
@@ -4044,27 +4036,27 @@
         <v>39</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C41" s="32">
         <v>3</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="F41" s="12"/>
       <c r="G41" s="12"/>
       <c r="H41" s="8" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="J41" s="11" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="K41" s="11" t="s">
         <v>13</v>
@@ -4073,10 +4065,10 @@
         <v>35</v>
       </c>
       <c r="M41" s="11" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="N41" s="11" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="210" x14ac:dyDescent="0.25">
@@ -4084,39 +4076,39 @@
         <v>40</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C42" s="32">
         <v>3</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="F42" s="12">
         <v>17</v>
       </c>
       <c r="G42" s="12"/>
       <c r="H42" s="8" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="J42" s="11" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="K42" s="20" t="s">
         <v>15</v>
       </c>
       <c r="L42" s="20"/>
       <c r="M42" s="11" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="N42" s="11" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="165" x14ac:dyDescent="0.25">
@@ -4124,39 +4116,39 @@
         <v>41</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C43" s="32">
         <v>3</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E43" s="11" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="F43" s="12">
         <v>17</v>
       </c>
       <c r="G43" s="12"/>
       <c r="H43" s="8" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="I43" s="8" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="J43" s="11" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="K43" s="20" t="s">
         <v>21</v>
       </c>
       <c r="L43" s="20"/>
       <c r="M43" s="11" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="N43" s="11" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="44" spans="1:14" s="1" customFormat="1" ht="180" x14ac:dyDescent="0.25">
@@ -4164,33 +4156,33 @@
         <v>42</v>
       </c>
       <c r="B44" s="27" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C44" s="50">
         <v>4</v>
       </c>
       <c r="D44" s="27" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E44" s="27" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="F44" s="28"/>
       <c r="G44" s="28"/>
       <c r="H44" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="J44" s="27"/>
       <c r="K44" s="29"/>
       <c r="L44" s="29"/>
       <c r="M44" s="30" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="N44" s="27" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="45" spans="1:14" s="1" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -4198,26 +4190,26 @@
         <v>43</v>
       </c>
       <c r="B45" s="27" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C45" s="50">
         <v>4</v>
       </c>
       <c r="D45" s="27" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E45" s="27" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="F45" s="28"/>
       <c r="G45" s="28" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="I45" s="8" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="J45" s="27"/>
       <c r="K45" s="29"/>
@@ -4225,10 +4217,10 @@
         <v>29</v>
       </c>
       <c r="M45" s="30" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="N45" s="27" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:14" s="41" customFormat="1" ht="180" x14ac:dyDescent="0.25">
@@ -4236,31 +4228,31 @@
         <v>44</v>
       </c>
       <c r="B46" s="38" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C46" s="40">
         <v>6</v>
       </c>
       <c r="D46" s="42" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="E46" s="42" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="F46" s="40"/>
       <c r="G46" s="40"/>
       <c r="H46" s="44" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="I46" s="44" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="J46" s="39"/>
       <c r="K46" s="39"/>
       <c r="L46" s="39"/>
       <c r="M46" s="38"/>
       <c r="N46" s="42" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="47" spans="1:14" s="41" customFormat="1" ht="225" x14ac:dyDescent="0.25">
@@ -4268,31 +4260,31 @@
         <v>45</v>
       </c>
       <c r="B47" s="38" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C47" s="40">
         <v>7</v>
       </c>
       <c r="D47" s="42" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="E47" s="42" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F47" s="40"/>
       <c r="G47" s="40"/>
       <c r="H47" s="44" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="I47" s="44" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="J47" s="39"/>
       <c r="K47" s="39"/>
       <c r="L47" s="39"/>
       <c r="M47" s="38"/>
       <c r="N47" s="42" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="48" spans="1:14" s="41" customFormat="1" ht="270" x14ac:dyDescent="0.25">
@@ -4300,31 +4292,31 @@
         <v>46</v>
       </c>
       <c r="B48" s="38" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C48" s="40">
         <v>8</v>
       </c>
       <c r="D48" s="42" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="E48" s="42" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="F48" s="40"/>
       <c r="G48" s="40"/>
       <c r="H48" s="44" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="I48" s="44" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="J48" s="39"/>
       <c r="K48" s="39"/>
       <c r="L48" s="39"/>
       <c r="M48" s="38"/>
       <c r="N48" s="42" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="49" spans="1:14" s="41" customFormat="1" ht="255" x14ac:dyDescent="0.25">
@@ -4332,31 +4324,31 @@
         <v>47</v>
       </c>
       <c r="B49" s="38" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C49" s="40">
         <v>9</v>
       </c>
       <c r="D49" s="42" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="E49" s="42" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="F49" s="40"/>
       <c r="G49" s="40"/>
       <c r="H49" s="44" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="I49" s="44" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="J49" s="39"/>
       <c r="K49" s="39"/>
       <c r="L49" s="39"/>
       <c r="M49" s="38"/>
       <c r="N49" s="42" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="50" spans="1:14" s="41" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -4364,31 +4356,31 @@
         <v>48</v>
       </c>
       <c r="B50" s="38" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C50" s="40">
         <v>10</v>
       </c>
       <c r="D50" s="42" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="E50" s="42" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="F50" s="40"/>
       <c r="G50" s="40"/>
       <c r="H50" s="44" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="I50" s="44" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="J50" s="39"/>
       <c r="K50" s="39"/>
       <c r="L50" s="39"/>
       <c r="M50" s="38"/>
       <c r="N50" s="45" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="51" spans="1:14" s="41" customFormat="1" ht="120" x14ac:dyDescent="0.25">
@@ -4396,31 +4388,31 @@
         <v>49</v>
       </c>
       <c r="B51" s="42" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C51" s="51">
         <v>11</v>
       </c>
       <c r="D51" s="42" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="E51" s="42" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="F51" s="40"/>
       <c r="G51" s="40"/>
       <c r="H51" s="44" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="I51" s="44" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="J51" s="39"/>
       <c r="K51" s="39"/>
       <c r="L51" s="39"/>
       <c r="M51" s="38"/>
       <c r="N51" s="42" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="52" spans="1:14" s="41" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -4428,31 +4420,31 @@
         <v>50</v>
       </c>
       <c r="B52" s="42" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C52" s="51">
         <v>12</v>
       </c>
       <c r="D52" s="42" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="E52" s="42" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="F52" s="40"/>
       <c r="G52" s="40"/>
       <c r="H52" s="44" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="I52" s="44" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="J52" s="39"/>
       <c r="K52" s="39"/>
       <c r="L52" s="39"/>
       <c r="M52" s="38"/>
       <c r="N52" s="42" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="53" spans="1:14" s="41" customFormat="1" ht="165" x14ac:dyDescent="0.25">
@@ -4460,31 +4452,31 @@
         <v>51</v>
       </c>
       <c r="B53" s="38" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="C53" s="40">
         <v>13</v>
       </c>
       <c r="D53" s="42" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="E53" s="42" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="F53" s="40"/>
       <c r="G53" s="40"/>
       <c r="H53" s="44" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="I53" s="44" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="J53" s="39"/>
       <c r="K53" s="39"/>
       <c r="L53" s="39"/>
       <c r="M53" s="38"/>
       <c r="N53" s="45" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="54" spans="1:14" s="41" customFormat="1" ht="210" x14ac:dyDescent="0.25">
@@ -4492,31 +4484,31 @@
         <v>52</v>
       </c>
       <c r="B54" s="42" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="C54" s="51">
         <v>14</v>
       </c>
       <c r="D54" s="42" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="E54" s="42" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="F54" s="40"/>
       <c r="G54" s="40"/>
       <c r="H54" s="44" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="I54" s="44" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="J54" s="39"/>
       <c r="K54" s="39"/>
       <c r="L54" s="39"/>
       <c r="M54" s="38"/>
       <c r="N54" s="42" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -4533,18 +4525,18 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="M35" r:id="rId1"/>
-    <hyperlink ref="M44" r:id="rId2" display="https://positivepsychology.com/thought-diary/"/>
-    <hyperlink ref="M45" r:id="rId3" display="https://www.stichtingstopbewust.nl/_x000a__x000a_Michie, S., Ashford, S., Sniehotta, FalkoF., Dombrowski, StephanU., Bishop, A., &amp; French, DavidP. (2011). A refined taxonomy of behaviour change techniques to help people change their physical activity and healthy eating behaviours: The CALO-RE taxonomy. Psychology &amp; Health, 26(11), 1479–1498. https://doi.org/10.1080/08870446.2010.540664"/>
-    <hyperlink ref="M34" r:id="rId4"/>
-    <hyperlink ref="M36" r:id="rId5"/>
-    <hyperlink ref="M4" r:id="rId6"/>
-    <hyperlink ref="N4" r:id="rId7"/>
-    <hyperlink ref="N34" r:id="rId8"/>
-    <hyperlink ref="N35" r:id="rId9"/>
-    <hyperlink ref="N36" r:id="rId10"/>
-    <hyperlink ref="N50" r:id="rId11"/>
-    <hyperlink ref="N53" r:id="rId12" location=":~:text=It%20a%2021%2Ditem%20measure,recreational%20facilities%2C%20exercise%20equipment)"/>
+    <hyperlink ref="M35" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="M44" r:id="rId2" display="https://positivepsychology.com/thought-diary/" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="M45" r:id="rId3" display="https://www.stichtingstopbewust.nl/_x000a__x000a_Michie, S., Ashford, S., Sniehotta, FalkoF., Dombrowski, StephanU., Bishop, A., &amp; French, DavidP. (2011). A refined taxonomy of behaviour change techniques to help people change their physical activity and healthy eating behaviours: The CALO-RE taxonomy. Psychology &amp; Health, 26(11), 1479–1498. https://doi.org/10.1080/08870446.2010.540664" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="M34" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="M36" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="M4" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="N4" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="N34" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="N35" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="N36" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="N50" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="N53" r:id="rId12" location=":~:text=It%20a%2021%2Ditem%20measure,recreational%20facilities%2C%20exercise%20equipment)" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId13"/>

</xml_diff>